<commit_message>
added data set model map
</commit_message>
<xml_diff>
--- a/models-src/oah-models-and-maps.xlsx
+++ b/models-src/oah-models-and-maps.xlsx
@@ -8,43 +8,44 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\oah\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3A9103-68D5-47D8-9C43-922FA309DEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9A9BE0-1FEF-4791-8EEF-082A507C833B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" firstSheet="4" activeTab="7" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" firstSheet="4" activeTab="6" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
   <sheets>
     <sheet name="LogicalModels-bak" sheetId="53" r:id="rId1"/>
     <sheet name="IG-groups" sheetId="31" r:id="rId2"/>
     <sheet name="CodeSystem" sheetId="45" r:id="rId3"/>
     <sheet name="StructuredIndicatorOah2FHIR" sheetId="55" r:id="rId4"/>
-    <sheet name="SimpleIndicatorOah2FHIR" sheetId="34" r:id="rId5"/>
-    <sheet name="ConceptMaps" sheetId="17" r:id="rId6"/>
-    <sheet name="LogicalModels" sheetId="15" r:id="rId7"/>
-    <sheet name="DataSetOah" sheetId="56" r:id="rId8"/>
-    <sheet name="IndicatorsOah2FHIR" sheetId="54" r:id="rId9"/>
-    <sheet name="Sample" sheetId="48" r:id="rId10"/>
-    <sheet name="SampleOah" sheetId="49" r:id="rId11"/>
-    <sheet name="IndicatorsOah" sheetId="47" r:id="rId12"/>
-    <sheet name="IndicatorOah-bak" sheetId="50" r:id="rId13"/>
-    <sheet name="StructuredIndicatorOah" sheetId="52" r:id="rId14"/>
-    <sheet name="SimpleIndicatorOah" sheetId="51" r:id="rId15"/>
-    <sheet name="BioIndicatorsOah" sheetId="11" r:id="rId16"/>
-    <sheet name="HydroMorphIndicatorsOah" sheetId="39" r:id="rId17"/>
-    <sheet name="WaterIndicatorsOah" sheetId="42" r:id="rId18"/>
-    <sheet name="BioRisksIndicatorsOah" sheetId="44" r:id="rId19"/>
-    <sheet name="Foglio1" sheetId="37" r:id="rId20"/>
-    <sheet name="Foglio2" sheetId="38" r:id="rId21"/>
-    <sheet name="Foglio4" sheetId="40" r:id="rId22"/>
-    <sheet name="Foglio7" sheetId="43" r:id="rId23"/>
+    <sheet name="DataSetOah2FHIR" sheetId="57" r:id="rId5"/>
+    <sheet name="SimpleIndicatorOah2FHIR" sheetId="34" r:id="rId6"/>
+    <sheet name="ConceptMaps" sheetId="17" r:id="rId7"/>
+    <sheet name="LogicalModels" sheetId="15" r:id="rId8"/>
+    <sheet name="DataSetOah" sheetId="56" r:id="rId9"/>
+    <sheet name="IndicatorsOah2FHIR" sheetId="54" r:id="rId10"/>
+    <sheet name="Sample" sheetId="48" r:id="rId11"/>
+    <sheet name="SampleOah" sheetId="49" r:id="rId12"/>
+    <sheet name="IndicatorsOah" sheetId="47" r:id="rId13"/>
+    <sheet name="IndicatorOah-bak" sheetId="50" r:id="rId14"/>
+    <sheet name="StructuredIndicatorOah" sheetId="52" r:id="rId15"/>
+    <sheet name="SimpleIndicatorOah" sheetId="51" r:id="rId16"/>
+    <sheet name="BioIndicatorsOah" sheetId="11" r:id="rId17"/>
+    <sheet name="HydroMorphIndicatorsOah" sheetId="39" r:id="rId18"/>
+    <sheet name="WaterIndicatorsOah" sheetId="42" r:id="rId19"/>
+    <sheet name="BioRisksIndicatorsOah" sheetId="44" r:id="rId20"/>
+    <sheet name="Foglio1" sheetId="37" r:id="rId21"/>
+    <sheet name="Foglio2" sheetId="38" r:id="rId22"/>
+    <sheet name="Foglio4" sheetId="40" r:id="rId23"/>
+    <sheet name="Foglio7" sheetId="43" r:id="rId24"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId24"/>
+    <externalReference r:id="rId25"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">BioRisksIndicatorsOah!$A$1:$E$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">DataSetOah!$A$1:$E$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">HydroMorphIndicatorsOah!$A$1:$E$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WaterIndicatorsOah!$A$1:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">BioRisksIndicatorsOah!$A$1:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">DataSetOah!$A$1:$E$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">HydroMorphIndicatorsOah!$A$1:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">WaterIndicatorsOah!$A$1:$E$4</definedName>
     <definedName name="CENEN13606Lekarska_prepustacia_sprava">'[1]Hospital Discharge Report '!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="621">
   <si>
     <t>Group Source</t>
   </si>
@@ -2668,30 +2669,12 @@
     <t>publisher</t>
   </si>
   <si>
-    <t>Date of the last change</t>
-  </si>
-  <si>
     <t>version</t>
   </si>
   <si>
-    <t>dateOfLastChange</t>
-  </si>
-  <si>
-    <t>dateOfPublication</t>
-  </si>
-  <si>
-    <t>Date of publication</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
-    <t>Date o Publicaiton of the data set</t>
-  </si>
-  <si>
-    <t>Date of last update of the data in the data set</t>
-  </si>
-  <si>
     <t>Data set version</t>
   </si>
   <si>
@@ -2737,9 +2720,6 @@
     <t>record.title</t>
   </si>
   <si>
-    <t>record.description</t>
-  </si>
-  <si>
     <t>record.format</t>
   </si>
   <si>
@@ -2764,9 +2744,6 @@
     <t>Where the record can be accessed</t>
   </si>
   <si>
-    <t>Record Description</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
@@ -2807,6 +2784,129 @@
   </si>
   <si>
     <t>globally uniqu,  persistent and resolvable identifier</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/ig/oah/StructureDefinition/library-oah</t>
+  </si>
+  <si>
+    <t>Library.url</t>
+  </si>
+  <si>
+    <t>Library.title</t>
+  </si>
+  <si>
+    <t>Library.copyright</t>
+  </si>
+  <si>
+    <t>Library.description</t>
+  </si>
+  <si>
+    <t>Library.version</t>
+  </si>
+  <si>
+    <t>Library.type</t>
+  </si>
+  <si>
+    <t>Library.contact</t>
+  </si>
+  <si>
+    <t>Library.publisher</t>
+  </si>
+  <si>
+    <t>Library.author</t>
+  </si>
+  <si>
+    <t>Library.date</t>
+  </si>
+  <si>
+    <t>Library.lastReviewDate</t>
+  </si>
+  <si>
+    <t>Data set Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The date when the data set was last significantly changed. </t>
+  </si>
+  <si>
+    <t>dateOfReview</t>
+  </si>
+  <si>
+    <t>Date of last review</t>
+  </si>
+  <si>
+    <t>The date on which the resource content was last reviewed. Review happens periodically after approval but does not change the original approval date.</t>
+  </si>
+  <si>
+    <t>dateOfApproval</t>
+  </si>
+  <si>
+    <t>Date of approval</t>
+  </si>
+  <si>
+    <t>When the publisher approaved the data set for publication</t>
+  </si>
+  <si>
+    <t>Library.approvalDate</t>
+  </si>
+  <si>
+    <t>Library.extension[licence]</t>
+  </si>
+  <si>
+    <t>extension[size].valueQuantity</t>
+  </si>
+  <si>
+    <t>extension[numberOfRecords].valueInteger</t>
+  </si>
+  <si>
+    <t>Library.content</t>
+  </si>
+  <si>
+    <t>extension[copyrightLabel].valueString</t>
+  </si>
+  <si>
+    <t>Attachment</t>
+  </si>
+  <si>
+    <t>Attachment.title</t>
+  </si>
+  <si>
+    <t>Attachment.contentType</t>
+  </si>
+  <si>
+    <t>Attachment.url</t>
+  </si>
+  <si>
+    <t>Attachment.size</t>
+  </si>
+  <si>
+    <t>Library.dataRequirement</t>
+  </si>
+  <si>
+    <t>DataRequirement</t>
+  </si>
+  <si>
+    <t>DataRequirement.type</t>
+  </si>
+  <si>
+    <t>as MIME type</t>
+  </si>
+  <si>
+    <t>As FHIR resource</t>
+  </si>
+  <si>
+    <t>DataRequirement.profile</t>
+  </si>
+  <si>
+    <t>As FHIR profile</t>
+  </si>
+  <si>
+    <t>DataSetOah2FHIR</t>
+  </si>
+  <si>
+    <t>OAH Data Set Model to this guide Map</t>
+  </si>
+  <si>
+    <t>OAH Data Set Model to this guide mapping</t>
   </si>
 </sst>
 </file>
@@ -3095,7 +3195,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3292,6 +3392,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -3837,6 +3941,880 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08DA2C3-843D-4662-B2C7-78EB4A1DCF4E}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75"/>
+  <cols>
+    <col min="1" max="1" width="58.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.86328125" customWidth="1"/>
+    <col min="3" max="3" width="76.81640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.2265625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="11.1328125" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="14" customFormat="1">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C2" s="8" t="str">
+        <f>IndicatorsOah!A2</f>
+        <v>biological</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>IndicatorsOah!D2</f>
+        <v>Key biological quality indicators</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" ht="29.5">
+      <c r="A3" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" s="8" t="str">
+        <f>IndicatorsOah!A3</f>
+        <v>biological.macroinvertebreates</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>IndicatorsOah!D3</f>
+        <v>Benthic Macroinvertebrates</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="6" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C4" s="8" t="str">
+        <f>IndicatorsOah!A4</f>
+        <v>biological.diatomes</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f>IndicatorsOah!D4</f>
+        <v>Diatoms (microalgae/phytobenthos)</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C5" s="8" t="str">
+        <f>IndicatorsOah!A5</f>
+        <v>biological.fishes</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f>IndicatorsOah!D5</f>
+        <v>Fish</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="44.25">
+      <c r="A6" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="C6" s="8" t="str">
+        <f>IndicatorsOah!A6</f>
+        <v>biological.macrophytes</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f>IndicatorsOah!D6</f>
+        <v>Macrophytes (aquatic plants)</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="44.25">
+      <c r="A7" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>IndicatorsOah!A7</f>
+        <v>biological.riparianVegetation</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f>IndicatorsOah!D7</f>
+        <v>Riparian vegetation</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C8" s="8" t="str">
+        <f>IndicatorsOah!A8</f>
+        <v>biological.microbiomes</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>IndicatorsOah!D8</f>
+        <v>Microbiomes/Biofilms</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>IndicatorsOah!A9</f>
+        <v>hydromorphological</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>IndicatorsOah!D9</f>
+        <v>Key hydromorphological quality indicators</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C10" s="8" t="str">
+        <f>IndicatorsOah!A10</f>
+        <v>hydromorphological.morphology</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>IndicatorsOah!D10</f>
+        <v>Morphology of the streams</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C11" s="8" t="str">
+        <f>IndicatorsOah!A11</f>
+        <v>hydromorphological.hydrology</v>
+      </c>
+      <c r="D11" s="8" t="str">
+        <f>IndicatorsOah!D11</f>
+        <v>Hydrology of the stream</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C12" s="8" t="str">
+        <f>IndicatorsOah!A12</f>
+        <v>hydromorphological.landUse</v>
+      </c>
+      <c r="D12" s="8" t="str">
+        <f>IndicatorsOah!D12</f>
+        <v>Land use in the margins</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C13" s="8" t="str">
+        <f>IndicatorsOah!A13</f>
+        <v>water</v>
+      </c>
+      <c r="D13" s="8" t="str">
+        <f>IndicatorsOah!D13</f>
+        <v>Key water quality indicators</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C14" s="8" t="str">
+        <f>IndicatorsOah!A14</f>
+        <v>water.nutrients</v>
+      </c>
+      <c r="D14" s="8" t="str">
+        <f>IndicatorsOah!D14</f>
+        <v>Nutrients</v>
+      </c>
+      <c r="E14" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C15" s="8" t="str">
+        <f>IndicatorsOah!A15</f>
+        <v>water.pH</v>
+      </c>
+      <c r="D15" s="8" t="str">
+        <f>IndicatorsOah!D15</f>
+        <v>pH</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C16" s="8" t="str">
+        <f>IndicatorsOah!A16</f>
+        <v>water.dissolvedO2</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <f>IndicatorsOah!D16</f>
+        <v>Dissolved O2</v>
+      </c>
+      <c r="E16" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="29.5">
+      <c r="A17" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C17" s="8" t="str">
+        <f>IndicatorsOah!A17</f>
+        <v>water.waterTemperature</v>
+      </c>
+      <c r="D17" s="8" t="str">
+        <f>IndicatorsOah!D17</f>
+        <v>Water temperature</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C18" s="8" t="str">
+        <f>IndicatorsOah!A18</f>
+        <v>water.tds</v>
+      </c>
+      <c r="D18" s="8" t="str">
+        <f>IndicatorsOah!D18</f>
+        <v>Total dissolved solids (TDS)</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C19" s="8" t="str">
+        <f>IndicatorsOah!A19</f>
+        <v>water.tss</v>
+      </c>
+      <c r="D19" s="8" t="str">
+        <f>IndicatorsOah!D19</f>
+        <v>Total suspended solids (TSS)</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C20" s="8" t="str">
+        <f>IndicatorsOah!A20</f>
+        <v>water.conductivity</v>
+      </c>
+      <c r="D20" s="8" t="str">
+        <f>IndicatorsOah!D20</f>
+        <v>Conductivity</v>
+      </c>
+      <c r="E20" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="29.5">
+      <c r="A21" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C21" s="8" t="str">
+        <f>IndicatorsOah!A21</f>
+        <v>water.pharmaceuticals</v>
+      </c>
+      <c r="D21" s="8" t="str">
+        <f>IndicatorsOah!D21</f>
+        <v>Pharmaceuticals</v>
+      </c>
+      <c r="E21" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C22" s="8" t="str">
+        <f>IndicatorsOah!A22</f>
+        <v>water.foam</v>
+      </c>
+      <c r="D22" s="8" t="str">
+        <f>IndicatorsOah!D22</f>
+        <v>Foam/colour/smell</v>
+      </c>
+      <c r="E22" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C23" s="8" t="str">
+        <f>IndicatorsOah!A23</f>
+        <v>water.coliforms</v>
+      </c>
+      <c r="D23" s="8" t="str">
+        <f>IndicatorsOah!D23</f>
+        <v>Coliforms</v>
+      </c>
+      <c r="E23" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C24" s="8" t="str">
+        <f>IndicatorsOah!A24</f>
+        <v>bioRisk</v>
+      </c>
+      <c r="D24" s="8" t="str">
+        <f>IndicatorsOah!D24</f>
+        <v>Biological indicators of health risks</v>
+      </c>
+      <c r="E24" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C25" s="8" t="str">
+        <f>IndicatorsOah!A25</f>
+        <v>bioRisk.diptera</v>
+      </c>
+      <c r="D25" s="8" t="str">
+        <f>IndicatorsOah!D25</f>
+        <v>Diptera</v>
+      </c>
+      <c r="E25" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C26" s="8" t="str">
+        <f>IndicatorsOah!A26</f>
+        <v>bioRisk.ticks</v>
+      </c>
+      <c r="D26" s="8" t="str">
+        <f>IndicatorsOah!D26</f>
+        <v>Ticks</v>
+      </c>
+      <c r="E26" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="29.5">
+      <c r="A27" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C27" s="8" t="str">
+        <f>IndicatorsOah!A27</f>
+        <v>bioRisk.invasiveOrganisms</v>
+      </c>
+      <c r="D27" s="8" t="str">
+        <f>IndicatorsOah!D27</f>
+        <v>Invasive invertebrate, plants and fish</v>
+      </c>
+      <c r="E27" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C28" s="8" t="str">
+        <f>IndicatorsOah!A28</f>
+        <v>bioRisk.birds</v>
+      </c>
+      <c r="D28" s="8" t="str">
+        <f>IndicatorsOah!D28</f>
+        <v>Birds</v>
+      </c>
+      <c r="E28" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="29.5">
+      <c r="A29" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C29" s="8" t="str">
+        <f>IndicatorsOah!A29</f>
+        <v>bioRisk.diatomTratology</v>
+      </c>
+      <c r="D29" s="8" t="str">
+        <f>IndicatorsOah!D29</f>
+        <v>Diatom teratology</v>
+      </c>
+      <c r="E29" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C30" s="8" t="str">
+        <f>IndicatorsOah!A30</f>
+        <v>bioRisk.fish</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f>IndicatorsOah!D30</f>
+        <v>Fish</v>
+      </c>
+      <c r="E30" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C31" s="8" t="str">
+        <f>IndicatorsOah!A31</f>
+        <v>bioRisk.amphibians</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f>IndicatorsOah!D31</f>
+        <v>Amphibians</v>
+      </c>
+      <c r="E31" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{59D91ED4-2DF1-4999-9702-333D5B4701FB}"/>
+    <hyperlink ref="A1" r:id="rId2" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{7243FA7D-51BD-482B-BCBD-549089E492AF}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{BEE4E2F4-063C-4DFF-82C5-B6626E4B1A4E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A488BF-AD8E-4BE5-A39A-DE3C1860562E}">
   <dimension ref="A2:K53"/>
   <sheetViews>
@@ -4144,7 +5122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E1E018-F3BA-4B95-9856-259080B6D3DC}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -4319,7 +5297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA67BB8F-F241-4238-A116-030260AF1676}">
   <dimension ref="A1:E31"/>
   <sheetViews>
@@ -4868,7 +5846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ED8D9E-4C8F-4866-AD65-D95CCFA6E5A0}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -5043,7 +6021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8B5A90-6D36-45B7-9347-AA4594F3DFDD}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -5201,7 +6179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8917C38-1E9C-4CA8-B026-1EC7F0AF7FE1}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -5325,7 +6303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
@@ -5724,7 +6702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4D5EE3-E5BC-48B0-8772-0AA9839A90B5}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
@@ -5818,7 +6796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C83865-7D7A-4AB5-950B-27F95F3290B9}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
@@ -6044,7 +7022,179 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BB872A-9AFB-4D24-BD9C-EB65B5EB34C4}">
+  <dimension ref="B9:B38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:B35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetData>
+    <row r="9" spans="2:2">
+      <c r="B9" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="e">
+        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="str">
+        <f>"- ConceptMap/"&amp;ConceptMaps!A2</f>
+        <v>- ConceptMap/IndicatorsOah2FHIR</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="str">
+        <f>"- ConceptMap/"&amp;ConceptMaps!A3</f>
+        <v>- ConceptMap/SimpleIndicatorOah2FHIR</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="str">
+        <f>"- ConceptMap/"&amp;ConceptMaps!A4</f>
+        <v>- ConceptMap/StructuredIndicatorOah2FHIR</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="str">
+        <f>"- ConceptMap/"&amp;ConceptMaps!A5</f>
+        <v>- ConceptMap/DataSetOah2FHIR</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="str">
+        <f>"- ConceptMap/"&amp;ConceptMaps!A6</f>
+        <v>- ConceptMap/</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="str">
+        <f>"- ConceptMap/"&amp;ConceptMaps!A7</f>
+        <v>- ConceptMap/</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="str">
+        <f>"- ConceptMap/"&amp;ConceptMaps!A8</f>
+        <v>- ConceptMap/</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="str">
+        <f>"- ConceptMap/"&amp;ConceptMaps!A9</f>
+        <v>- ConceptMap/</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="str">
+        <f>"- ConceptMap/"&amp;ConceptMaps!A10</f>
+        <v>- ConceptMap/</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="str">
+        <f>"- ConceptMap/"&amp;ConceptMaps!A11</f>
+        <v>- ConceptMap/</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="str">
+        <f>"- ConceptMap/"&amp;ConceptMaps!A12</f>
+        <v>- ConceptMap/</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD48B1E5-E78A-4640-8685-256B624A7564}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
@@ -6222,179 +7372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BB872A-9AFB-4D24-BD9C-EB65B5EB34C4}">
-  <dimension ref="B9:B38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:B35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
-  <sheetData>
-    <row r="9" spans="2:2">
-      <c r="B9" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
-      <c r="B10" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2">
-      <c r="B11" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2">
-      <c r="B12" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2">
-      <c r="B13" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2">
-      <c r="B14" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2">
-      <c r="B15" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2">
-      <c r="B16" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="e">
-        <f>"- StructureDefinition/"&amp;LogicalModels!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" t="str">
-        <f>"- ConceptMap/"&amp;ConceptMaps!A2</f>
-        <v>- ConceptMap/IndicatorsOah2FHIR</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" t="str">
-        <f>"- ConceptMap/"&amp;ConceptMaps!A3</f>
-        <v>- ConceptMap/SimpleIndicatorOah2FHIR</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2">
-      <c r="B30" t="str">
-        <f>"- ConceptMap/"&amp;ConceptMaps!A4</f>
-        <v>- ConceptMap/StructuredIndicatorOah2FHIR</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" t="str">
-        <f>"- ConceptMap/"&amp;ConceptMaps!A5</f>
-        <v>- ConceptMap/</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" t="str">
-        <f>"- ConceptMap/"&amp;ConceptMaps!A6</f>
-        <v>- ConceptMap/</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="str">
-        <f>"- ConceptMap/"&amp;ConceptMaps!A7</f>
-        <v>- ConceptMap/</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" t="str">
-        <f>"- ConceptMap/"&amp;ConceptMaps!A8</f>
-        <v>- ConceptMap/</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" t="str">
-        <f>"- ConceptMap/"&amp;ConceptMaps!A9</f>
-        <v>- ConceptMap/</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" t="str">
-        <f>"- ConceptMap/"&amp;ConceptMaps!A10</f>
-        <v>- ConceptMap/</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" t="str">
-        <f>"- ConceptMap/"&amp;ConceptMaps!A11</f>
-        <v>- ConceptMap/</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" t="str">
-        <f>"- ConceptMap/"&amp;ConceptMaps!A12</f>
-        <v>- ConceptMap/</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2A7343-37D8-40E6-B2E1-BBF761782857}">
   <dimension ref="A1:E56"/>
   <sheetViews>
@@ -7049,7 +8027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91AD1C54-3000-446F-8B7A-1DB26DD07144}">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -7296,7 +8274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D66D59-188A-4C35-BC92-8A254DC4CBFA}">
   <dimension ref="A1:E29"/>
   <sheetViews>
@@ -7676,7 +8654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4375491-B056-4D0F-9FBA-CE54A9A308DA}">
   <dimension ref="A1:E37"/>
   <sheetViews>
@@ -8908,6 +9886,698 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CAA406-B92E-4F33-947E-7872EDD03684}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75"/>
+  <cols>
+    <col min="1" max="1" width="58.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.86328125" customWidth="1"/>
+    <col min="3" max="3" width="36.04296875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.2265625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="11.1328125" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="14" customFormat="1">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29.5">
+      <c r="A2" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C2" s="8" t="str">
+        <f>DataSetOah!A2</f>
+        <v>pid</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>DataSetOah!D2</f>
+        <v>globally uniqu,  persistent and resolvable identifier</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C3" s="8" t="str">
+        <f>DataSetOah!A3</f>
+        <v>title</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>DataSetOah!D3</f>
+        <v>Data set title</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C4" s="8" t="str">
+        <f>DataSetOah!A4</f>
+        <v>description</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f>DataSetOah!D4</f>
+        <v>Data set desxription</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>584</v>
+      </c>
+      <c r="F4" s="6" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C5" s="8" t="str">
+        <f>DataSetOah!A5</f>
+        <v>version</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f>DataSetOah!D5</f>
+        <v>Data set version</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="F5" s="6" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C6" s="8" t="str">
+        <f>DataSetOah!A6</f>
+        <v>type</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f>DataSetOah!D6</f>
+        <v>Data Set type</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>586</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>DataSetOah!A7</f>
+        <v>contact</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f>DataSetOah!D7</f>
+        <v>Contact details</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C8" s="8" t="str">
+        <f>DataSetOah!A8</f>
+        <v>publisher</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>DataSetOah!D8</f>
+        <v>Data Set publisher</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>588</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>DataSetOah!A9</f>
+        <v>author</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>DataSetOah!D9</f>
+        <v>Data Set Author(s)</v>
+      </c>
+      <c r="E9" s="78" t="s">
+        <v>589</v>
+      </c>
+      <c r="G9" s="79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C10" s="8" t="str">
+        <f>DataSetOah!A10</f>
+        <v>date</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>DataSetOah!D10</f>
+        <v>Data set Date</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C11" s="8" t="str">
+        <f>DataSetOah!A11</f>
+        <v>dateOfApproval</v>
+      </c>
+      <c r="D11" s="8" t="str">
+        <f>DataSetOah!D11</f>
+        <v>Date of approval</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>600</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C12" s="8" t="str">
+        <f>DataSetOah!A12</f>
+        <v>dateOfReview</v>
+      </c>
+      <c r="D12" s="8" t="str">
+        <f>DataSetOah!D12</f>
+        <v>Date of last review</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C13" s="8" t="str">
+        <f>DataSetOah!A13</f>
+        <v>licence</v>
+      </c>
+      <c r="D13" s="8" t="str">
+        <f>DataSetOah!D13</f>
+        <v>licence information</v>
+      </c>
+      <c r="E13" s="74" t="s">
+        <v>601</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C14" s="8" t="str">
+        <f>DataSetOah!A14</f>
+        <v>copyright</v>
+      </c>
+      <c r="D14" s="8" t="str">
+        <f>DataSetOah!D14</f>
+        <v>Data set copyright</v>
+      </c>
+      <c r="E14" s="74" t="s">
+        <v>605</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C15" s="8" t="str">
+        <f>DataSetOah!A14</f>
+        <v>copyright</v>
+      </c>
+      <c r="D15" s="8" t="str">
+        <f>DataSetOah!D14</f>
+        <v>Data set copyright</v>
+      </c>
+      <c r="E15" s="74" t="s">
+        <v>583</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C16" s="8" t="str">
+        <f>DataSetOah!A15</f>
+        <v>size</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <f>DataSetOah!D15</f>
+        <v>Data set size</v>
+      </c>
+      <c r="E16" s="74" t="s">
+        <v>602</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C17" s="8" t="str">
+        <f>DataSetOah!A16</f>
+        <v>numberOfRecords</v>
+      </c>
+      <c r="D17" s="8" t="str">
+        <f>DataSetOah!D16</f>
+        <v>Number of records</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C18" s="8" t="str">
+        <f>DataSetOah!A17</f>
+        <v>record</v>
+      </c>
+      <c r="D18" s="8" t="str">
+        <f>DataSetOah!D17</f>
+        <v>record in the dat set</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="C19" s="8" t="str">
+        <f>DataSetOah!A18</f>
+        <v>record.title</v>
+      </c>
+      <c r="D19" s="8" t="str">
+        <f>DataSetOah!D18</f>
+        <v>Title</v>
+      </c>
+      <c r="E19" s="74" t="s">
+        <v>607</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="C20" s="8" t="str">
+        <f>DataSetOah!A19</f>
+        <v>record.format</v>
+      </c>
+      <c r="D20" s="8" t="str">
+        <f>DataSetOah!D19</f>
+        <v>Format</v>
+      </c>
+      <c r="E20" s="74" t="s">
+        <v>608</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="C21" s="8" t="str">
+        <f>DataSetOah!A20</f>
+        <v>record.link</v>
+      </c>
+      <c r="D21" s="8" t="str">
+        <f>DataSetOah!D20</f>
+        <v>Link</v>
+      </c>
+      <c r="E21" s="74" t="s">
+        <v>609</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="C22" s="8" t="str">
+        <f>DataSetOah!A21</f>
+        <v>record.size</v>
+      </c>
+      <c r="D22" s="8" t="str">
+        <f>DataSetOah!D21</f>
+        <v>Size</v>
+      </c>
+      <c r="E22" s="74" t="s">
+        <v>610</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C23" s="8" t="str">
+        <f>DataSetOah!A19</f>
+        <v>record.format</v>
+      </c>
+      <c r="D23" s="8" t="str">
+        <f>DataSetOah!D19</f>
+        <v>Format</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="C24" s="8" t="str">
+        <f>DataSetOah!$A$19</f>
+        <v>record.format</v>
+      </c>
+      <c r="D24" s="8" t="str">
+        <f>DataSetOah!$D$19</f>
+        <v>Format</v>
+      </c>
+      <c r="E24" s="74" t="s">
+        <v>613</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="C25" s="8" t="str">
+        <f>DataSetOah!$A$19</f>
+        <v>record.format</v>
+      </c>
+      <c r="D25" s="8" t="str">
+        <f>DataSetOah!$D$19</f>
+        <v>Format</v>
+      </c>
+      <c r="E25" s="74" t="s">
+        <v>616</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>617</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4AF26D06-028C-4E44-BC85-3271FDD3C9BB}"/>
+    <hyperlink ref="A1" r:id="rId2" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{E181CF34-81EF-44E5-98B8-1A9E617A5F12}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{E0379A6E-06E8-4390-B220-0F5A01F7451D}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{C61324D0-925A-45AF-B416-050DCC36004D}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{2A0C28C5-36D3-44BC-AACE-538E83D37800}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{8D136F09-2E94-4857-83F5-DBB79E8CE5AD}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{9C276A13-02FD-4066-B2F5-EBB691A2AD9D}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{34FA671B-98E3-4565-AEF8-6234D8135168}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{D28B9F98-2C1E-41CC-AD40-525CE7798596}"/>
+    <hyperlink ref="B10" r:id="rId10" xr:uid="{CAB97FFA-A885-451C-BBD3-C82D86DF7B3C}"/>
+    <hyperlink ref="B11" r:id="rId11" xr:uid="{B0BC8FB2-E8D2-4E73-A1CE-CFC44D0A0481}"/>
+    <hyperlink ref="B12" r:id="rId12" xr:uid="{1187D971-62C1-4B14-A7B7-7B146CB91B5F}"/>
+    <hyperlink ref="B13" r:id="rId13" xr:uid="{51E3F30A-D41E-4607-96B0-F7E170651064}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{780CC8D5-D095-4AC3-89BC-547ECE85D3EE}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{223B9E1C-CE56-403C-88FE-4A4A9CE483DC}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{71E86565-D107-41BB-90EC-3B0E7DEB8D70}"/>
+    <hyperlink ref="B14" r:id="rId17" xr:uid="{6C7449A5-9A5C-4740-962D-71674FB87125}"/>
+    <hyperlink ref="B15" r:id="rId18" xr:uid="{82CFA252-A51D-4400-B8F4-6E78DEDFD7F2}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{6CAAAF72-3777-4D31-84BC-530A0BC2DB49}"/>
+    <hyperlink ref="B24" r:id="rId20" location="DataRequirement" display="https://hl7.org/fhir/metadatatypes.html - DataRequirement" xr:uid="{B36472F0-D0AF-41FC-8B61-049644C82D8D}"/>
+    <hyperlink ref="B25" r:id="rId21" location="DataRequirement" display="https://hl7.org/fhir/metadatatypes.html - DataRequirement" xr:uid="{B86B98F1-80F1-44E7-A4BB-296CBD534A2A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B580CB-20F4-4431-9AC1-C7F103128FA7}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
@@ -9152,15 +10822,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E360F00-2125-41DA-88F8-A79DC0B018FC}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:AZ26"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
@@ -9362,10 +11032,25 @@
       <c r="AZ4"/>
     </row>
     <row r="5" spans="1:52" s="6" customFormat="1">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="A5" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="C5" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/ConceptMap/"&amp;A5</f>
+        <v>http://hl7.eu/fhir/ig/oah/ConceptMap/DataSetOah2FHIR</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>619</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="H5" s="10"/>
       <c r="J5"/>
       <c r="K5"/>
@@ -9601,13 +11286,14 @@
     <hyperlink ref="C3" r:id="rId2" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{58F1EE10-6CF4-4F90-8955-DEC223F5E5A1}"/>
     <hyperlink ref="C4" r:id="rId3" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{51D72151-E063-40DE-90B6-1578D72BDB4B}"/>
     <hyperlink ref="B4" location="StructuredIndicatorOah2FHIR!A1" display="StructuredIndicatorOah2FHIR" xr:uid="{56C6338D-D9FC-4776-92DC-9FD78F437E18}"/>
+    <hyperlink ref="C5" r:id="rId4" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{BF0DB1E2-0F2B-4E3E-805E-1CE18721AADF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -9695,16 +11381,16 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="D6" s="74" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
     </row>
   </sheetData>
@@ -9719,12 +11405,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31B2C70-17A7-40F9-AE47-E4872DBEC665}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A10" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
@@ -9756,7 +11442,7 @@
     </row>
     <row r="2" spans="1:5" ht="29.5">
       <c r="A2" s="75" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>394</v>
@@ -9765,10 +11451,10 @@
         <v>537</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -9779,13 +11465,13 @@
         <v>322</v>
       </c>
       <c r="C3" s="70" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -9796,30 +11482,30 @@
         <v>14</v>
       </c>
       <c r="C4" s="70" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="75" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>322</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="E5" s="39" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -9833,15 +11519,15 @@
         <v>417</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="75" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>14</v>
@@ -9850,10 +11536,10 @@
         <v>538</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -9864,13 +11550,13 @@
         <v>322</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -9890,9 +11576,9 @@
         <v>539</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="29.5">
       <c r="A10" s="75" t="s">
-        <v>544</v>
+        <v>372</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>322</v>
@@ -9901,15 +11587,15 @@
         <v>405</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>545</v>
+        <v>592</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>547</v>
+        <v>593</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29.5">
-      <c r="A11" s="76" t="s">
-        <v>543</v>
+      <c r="A11" s="75" t="s">
+        <v>597</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>322</v>
@@ -9918,168 +11604,168 @@
         <v>405</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>541</v>
+        <v>598</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="75" t="s">
-        <v>522</v>
+        <v>599</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="59">
+      <c r="A12" s="76" t="s">
+        <v>594</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>14</v>
+        <v>322</v>
       </c>
       <c r="C12" s="70" t="s">
-        <v>550</v>
+        <v>405</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>554</v>
+        <v>595</v>
       </c>
       <c r="E12" s="39" t="s">
-        <v>554</v>
+        <v>596</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="75" t="s">
-        <v>556</v>
+        <v>522</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="70" t="s">
+        <v>544</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>548</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="75" t="s">
         <v>550</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>544</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C15" s="70" t="s">
+        <v>425</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>551</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="B16" s="70" t="s">
+        <v>322</v>
+      </c>
+      <c r="C16" s="70" t="s">
+        <v>546</v>
+      </c>
+      <c r="D16" s="71" t="s">
+        <v>554</v>
+      </c>
+      <c r="E16" s="71" t="s">
         <v>555</v>
       </c>
-      <c r="E13" s="39" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C14" s="70" t="s">
-        <v>425</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>557</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="6" t="s">
-        <v>551</v>
-      </c>
-      <c r="B15" s="70" t="s">
-        <v>322</v>
-      </c>
-      <c r="C15" s="70" t="s">
-        <v>552</v>
-      </c>
-      <c r="D15" s="71" t="s">
-        <v>560</v>
-      </c>
-      <c r="E15" s="71" t="s">
+    </row>
+    <row r="17" spans="1:5" s="47" customFormat="1">
+      <c r="A17" s="75" t="s">
+        <v>556</v>
+      </c>
+      <c r="B17" s="75" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="77" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" s="47" customFormat="1">
-      <c r="A16" s="75" t="s">
-        <v>562</v>
-      </c>
-      <c r="B16" s="75" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="75" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="77" t="s">
-        <v>568</v>
-      </c>
-      <c r="E16" s="77" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="72" t="s">
-        <v>563</v>
-      </c>
-      <c r="B17" s="70" t="s">
-        <v>322</v>
-      </c>
-      <c r="C17" s="70" t="s">
-        <v>550</v>
-      </c>
-      <c r="D17" s="72" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="71" t="s">
-        <v>569</v>
+      <c r="E17" s="77" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="72" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="B18" s="70" t="s">
         <v>322</v>
       </c>
       <c r="C18" s="70" t="s">
-        <v>550</v>
-      </c>
-      <c r="D18" s="71" t="s">
-        <v>19</v>
+        <v>544</v>
+      </c>
+      <c r="D18" s="72" t="s">
+        <v>18</v>
       </c>
       <c r="E18" s="71" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="72" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="B19" s="70" t="s">
         <v>322</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D19" s="72" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="E19" s="71" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="72" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="B20" s="70" t="s">
         <v>322</v>
       </c>
       <c r="C20" s="70" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D20" s="72" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="E20" s="71" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="73" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="B21" s="70" t="s">
         <v>322</v>
@@ -10088,888 +11774,14 @@
         <v>425</v>
       </c>
       <c r="D21" s="73" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="E21" s="71" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E9" xr:uid="{FD4D5EE3-E5BC-48B0-8772-0AA9839A90B5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08DA2C3-843D-4662-B2C7-78EB4A1DCF4E}">
-  <sheetPr>
-    <tabColor theme="7" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:H34"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
-  <cols>
-    <col min="1" max="1" width="58.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.86328125" customWidth="1"/>
-    <col min="3" max="3" width="76.81640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.2265625" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="11.1328125" customWidth="1"/>
-    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C2" s="8" t="str">
-        <f>IndicatorsOah!A2</f>
-        <v>biological</v>
-      </c>
-      <c r="D2" s="8" t="str">
-        <f>IndicatorsOah!D2</f>
-        <v>Key biological quality indicators</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" ht="29.5">
-      <c r="A3" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C3" s="8" t="str">
-        <f>IndicatorsOah!A3</f>
-        <v>biological.macroinvertebreates</v>
-      </c>
-      <c r="D3" s="8" t="str">
-        <f>IndicatorsOah!D3</f>
-        <v>Benthic Macroinvertebrates</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="6" t="str">
-        <f>""</f>
-        <v/>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C4" s="8" t="str">
-        <f>IndicatorsOah!A4</f>
-        <v>biological.diatomes</v>
-      </c>
-      <c r="D4" s="8" t="str">
-        <f>IndicatorsOah!D4</f>
-        <v>Diatoms (microalgae/phytobenthos)</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C5" s="8" t="str">
-        <f>IndicatorsOah!A5</f>
-        <v>biological.fishes</v>
-      </c>
-      <c r="D5" s="8" t="str">
-        <f>IndicatorsOah!D5</f>
-        <v>Fish</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="44.25">
-      <c r="A6" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>472</v>
-      </c>
-      <c r="C6" s="8" t="str">
-        <f>IndicatorsOah!A6</f>
-        <v>biological.macrophytes</v>
-      </c>
-      <c r="D6" s="8" t="str">
-        <f>IndicatorsOah!D6</f>
-        <v>Macrophytes (aquatic plants)</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="44.25">
-      <c r="A7" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>472</v>
-      </c>
-      <c r="C7" s="8" t="str">
-        <f>IndicatorsOah!A7</f>
-        <v>biological.riparianVegetation</v>
-      </c>
-      <c r="D7" s="8" t="str">
-        <f>IndicatorsOah!D7</f>
-        <v>Riparian vegetation</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C8" s="8" t="str">
-        <f>IndicatorsOah!A8</f>
-        <v>biological.microbiomes</v>
-      </c>
-      <c r="D8" s="8" t="str">
-        <f>IndicatorsOah!D8</f>
-        <v>Microbiomes/Biofilms</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C9" s="8" t="str">
-        <f>IndicatorsOah!A9</f>
-        <v>hydromorphological</v>
-      </c>
-      <c r="D9" s="8" t="str">
-        <f>IndicatorsOah!D9</f>
-        <v>Key hydromorphological quality indicators</v>
-      </c>
-      <c r="E9" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C10" s="8" t="str">
-        <f>IndicatorsOah!A10</f>
-        <v>hydromorphological.morphology</v>
-      </c>
-      <c r="D10" s="8" t="str">
-        <f>IndicatorsOah!D10</f>
-        <v>Morphology of the streams</v>
-      </c>
-      <c r="E10" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C11" s="8" t="str">
-        <f>IndicatorsOah!A11</f>
-        <v>hydromorphological.hydrology</v>
-      </c>
-      <c r="D11" s="8" t="str">
-        <f>IndicatorsOah!D11</f>
-        <v>Hydrology of the stream</v>
-      </c>
-      <c r="E11" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C12" s="8" t="str">
-        <f>IndicatorsOah!A12</f>
-        <v>hydromorphological.landUse</v>
-      </c>
-      <c r="D12" s="8" t="str">
-        <f>IndicatorsOah!D12</f>
-        <v>Land use in the margins</v>
-      </c>
-      <c r="E12" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C13" s="8" t="str">
-        <f>IndicatorsOah!A13</f>
-        <v>water</v>
-      </c>
-      <c r="D13" s="8" t="str">
-        <f>IndicatorsOah!D13</f>
-        <v>Key water quality indicators</v>
-      </c>
-      <c r="E13" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C14" s="8" t="str">
-        <f>IndicatorsOah!A14</f>
-        <v>water.nutrients</v>
-      </c>
-      <c r="D14" s="8" t="str">
-        <f>IndicatorsOah!D14</f>
-        <v>Nutrients</v>
-      </c>
-      <c r="E14" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C15" s="8" t="str">
-        <f>IndicatorsOah!A15</f>
-        <v>water.pH</v>
-      </c>
-      <c r="D15" s="8" t="str">
-        <f>IndicatorsOah!D15</f>
-        <v>pH</v>
-      </c>
-      <c r="E15" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C16" s="8" t="str">
-        <f>IndicatorsOah!A16</f>
-        <v>water.dissolvedO2</v>
-      </c>
-      <c r="D16" s="8" t="str">
-        <f>IndicatorsOah!D16</f>
-        <v>Dissolved O2</v>
-      </c>
-      <c r="E16" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="29.5">
-      <c r="A17" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C17" s="8" t="str">
-        <f>IndicatorsOah!A17</f>
-        <v>water.waterTemperature</v>
-      </c>
-      <c r="D17" s="8" t="str">
-        <f>IndicatorsOah!D17</f>
-        <v>Water temperature</v>
-      </c>
-      <c r="E17" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C18" s="8" t="str">
-        <f>IndicatorsOah!A18</f>
-        <v>water.tds</v>
-      </c>
-      <c r="D18" s="8" t="str">
-        <f>IndicatorsOah!D18</f>
-        <v>Total dissolved solids (TDS)</v>
-      </c>
-      <c r="E18" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C19" s="8" t="str">
-        <f>IndicatorsOah!A19</f>
-        <v>water.tss</v>
-      </c>
-      <c r="D19" s="8" t="str">
-        <f>IndicatorsOah!D19</f>
-        <v>Total suspended solids (TSS)</v>
-      </c>
-      <c r="E19" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C20" s="8" t="str">
-        <f>IndicatorsOah!A20</f>
-        <v>water.conductivity</v>
-      </c>
-      <c r="D20" s="8" t="str">
-        <f>IndicatorsOah!D20</f>
-        <v>Conductivity</v>
-      </c>
-      <c r="E20" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="29.5">
-      <c r="A21" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C21" s="8" t="str">
-        <f>IndicatorsOah!A21</f>
-        <v>water.pharmaceuticals</v>
-      </c>
-      <c r="D21" s="8" t="str">
-        <f>IndicatorsOah!D21</f>
-        <v>Pharmaceuticals</v>
-      </c>
-      <c r="E21" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C22" s="8" t="str">
-        <f>IndicatorsOah!A22</f>
-        <v>water.foam</v>
-      </c>
-      <c r="D22" s="8" t="str">
-        <f>IndicatorsOah!D22</f>
-        <v>Foam/colour/smell</v>
-      </c>
-      <c r="E22" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C23" s="8" t="str">
-        <f>IndicatorsOah!A23</f>
-        <v>water.coliforms</v>
-      </c>
-      <c r="D23" s="8" t="str">
-        <f>IndicatorsOah!D23</f>
-        <v>Coliforms</v>
-      </c>
-      <c r="E23" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C24" s="8" t="str">
-        <f>IndicatorsOah!A24</f>
-        <v>bioRisk</v>
-      </c>
-      <c r="D24" s="8" t="str">
-        <f>IndicatorsOah!D24</f>
-        <v>Biological indicators of health risks</v>
-      </c>
-      <c r="E24" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C25" s="8" t="str">
-        <f>IndicatorsOah!A25</f>
-        <v>bioRisk.diptera</v>
-      </c>
-      <c r="D25" s="8" t="str">
-        <f>IndicatorsOah!D25</f>
-        <v>Diptera</v>
-      </c>
-      <c r="E25" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C26" s="8" t="str">
-        <f>IndicatorsOah!A26</f>
-        <v>bioRisk.ticks</v>
-      </c>
-      <c r="D26" s="8" t="str">
-        <f>IndicatorsOah!D26</f>
-        <v>Ticks</v>
-      </c>
-      <c r="E26" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="29.5">
-      <c r="A27" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C27" s="8" t="str">
-        <f>IndicatorsOah!A27</f>
-        <v>bioRisk.invasiveOrganisms</v>
-      </c>
-      <c r="D27" s="8" t="str">
-        <f>IndicatorsOah!D27</f>
-        <v>Invasive invertebrate, plants and fish</v>
-      </c>
-      <c r="E27" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C28" s="8" t="str">
-        <f>IndicatorsOah!A28</f>
-        <v>bioRisk.birds</v>
-      </c>
-      <c r="D28" s="8" t="str">
-        <f>IndicatorsOah!D28</f>
-        <v>Birds</v>
-      </c>
-      <c r="E28" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="29.5">
-      <c r="A29" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C29" s="8" t="str">
-        <f>IndicatorsOah!A29</f>
-        <v>bioRisk.diatomTratology</v>
-      </c>
-      <c r="D29" s="8" t="str">
-        <f>IndicatorsOah!D29</f>
-        <v>Diatom teratology</v>
-      </c>
-      <c r="E29" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C30" s="8" t="str">
-        <f>IndicatorsOah!A30</f>
-        <v>bioRisk.fish</v>
-      </c>
-      <c r="D30" s="8" t="str">
-        <f>IndicatorsOah!D30</f>
-        <v>Fish</v>
-      </c>
-      <c r="E30" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="C31" s="8" t="str">
-        <f>IndicatorsOah!A31</f>
-        <v>bioRisk.amphibians</v>
-      </c>
-      <c r="D31" s="8" t="str">
-        <f>IndicatorsOah!D31</f>
-        <v>Amphibians</v>
-      </c>
-      <c r="E31" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="3:3">
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="3:3">
-      <c r="C34" s="8"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{59D91ED4-2DF1-4999-9702-333D5B4701FB}"/>
-    <hyperlink ref="A1" r:id="rId2" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{7243FA7D-51BD-482B-BCBD-549089E492AF}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{BEE4E2F4-063C-4DFF-82C5-B6626E4B1A4E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added sample model to the IG; fixed links
</commit_message>
<xml_diff>
--- a/models-src/oah-models-and-maps.xlsx
+++ b/models-src/oah-models-and-maps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\oah\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555A70A8-CE2A-4D1E-B4A9-BE22760F7D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E281E1E6-71E7-4A88-A31F-66F09BA1B49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" firstSheet="6" activeTab="8" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
   <sheets>
     <sheet name="ConceptMaps" sheetId="17" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="315">
   <si>
     <t>Group Source</t>
   </si>
@@ -988,6 +988,15 @@
   </si>
   <si>
     <t>Location.extension[referenceForm]</t>
+  </si>
+  <si>
+    <t>SampleOah2FHIR</t>
+  </si>
+  <si>
+    <t>OAH Sample Model to this guide Map</t>
+  </si>
+  <si>
+    <t>OAH Sample Model to this guide mapping</t>
   </si>
 </sst>
 </file>
@@ -1619,8 +1628,8 @@
   </sheetPr>
   <dimension ref="A1:AZ26"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1823,20 +1832,20 @@
     </row>
     <row r="5" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A5" s="6" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/ConceptMap/"&amp;A5</f>
-        <v>http://hl7.eu/fhir/ig/oah/ConceptMap/DataSetOah2FHIR</v>
+        <v>http://hl7.eu/fhir/ig/oah/ConceptMap/SampleOah2FHIR</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>23</v>
@@ -1887,10 +1896,25 @@
       <c r="AZ5"/>
     </row>
     <row r="6" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="A6" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C6" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/ConceptMap/"&amp;A6</f>
+        <v>http://hl7.eu/fhir/ig/oah/ConceptMap/DataSetOah2FHIR</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="H6" s="10"/>
       <c r="J6"/>
       <c r="K6"/>
@@ -2076,11 +2100,12 @@
     <hyperlink ref="C3" r:id="rId2" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{58F1EE10-6CF4-4F90-8955-DEC223F5E5A1}"/>
     <hyperlink ref="C4" r:id="rId3" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{51D72151-E063-40DE-90B6-1578D72BDB4B}"/>
     <hyperlink ref="B4" location="StructuredIndicatorOah2FHIR!A1" display="StructuredIndicatorOah2FHIR" xr:uid="{56C6338D-D9FC-4776-92DC-9FD78F437E18}"/>
-    <hyperlink ref="C5" r:id="rId4" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{BF0DB1E2-0F2B-4E3E-805E-1CE18721AADF}"/>
-    <hyperlink ref="B5" location="DataSetOah2FHIR!A1" display="DataSetOah2FHIR" xr:uid="{269D91BA-A142-452C-BFC2-03E878D7FE34}"/>
+    <hyperlink ref="C6" r:id="rId4" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{BF0DB1E2-0F2B-4E3E-805E-1CE18721AADF}"/>
+    <hyperlink ref="B6" location="DataSetOah2FHIR!A1" display="DataSetOah2FHIR" xr:uid="{269D91BA-A142-452C-BFC2-03E878D7FE34}"/>
+    <hyperlink ref="C5" r:id="rId5" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{98932B28-070D-49A9-BFC9-E1569CC7F58A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -5880,7 +5905,7 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- Added remote.* block in IndicatorsOah (NDVI, EVI, NDWI, BWDRVI, NDCI, MCI) - Updated IndicatorsOah2FHIR mappings (with remote sensing indicators)
</commit_message>
<xml_diff>
--- a/models-src/oah-models-and-maps.xlsx
+++ b/models-src/oah-models-and-maps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\oah\models-src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\oah\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E281E1E6-71E7-4A88-A31F-66F09BA1B49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA00D202-8EFE-49FF-AD16-AA7F05CA57D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
   <sheets>
     <sheet name="ConceptMaps" sheetId="17" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="347">
   <si>
     <t>Group Source</t>
   </si>
@@ -997,6 +997,102 @@
   </si>
   <si>
     <t>OAH Sample Model to this guide mapping</t>
+  </si>
+  <si>
+    <t>remote</t>
+  </si>
+  <si>
+    <t>Remote sensing indices</t>
+  </si>
+  <si>
+    <t>Indices derived from satellite/UAV/airborne reflectance over water or riparian zones.</t>
+  </si>
+  <si>
+    <t>remote.ndci</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>Normalized Difference Chlorophyll Index (NDCI)</t>
+  </si>
+  <si>
+    <t>Index from multispectral reflectance indicating chlorophyll.</t>
+  </si>
+  <si>
+    <t>remote.mci</t>
+  </si>
+  <si>
+    <t>Maximum Chlorophyll Index (MCI)</t>
+  </si>
+  <si>
+    <t>index estimating high chlorophyll concentrations/blooms.</t>
+  </si>
+  <si>
+    <t>remote.bwdrvi</t>
+  </si>
+  <si>
+    <t>Blue Wide Dynamic Range Vegetation Index (BWDRVI)</t>
+  </si>
+  <si>
+    <t>Index  from blue/NIR; sensitive to aquatic vegetation/high biomass.</t>
+  </si>
+  <si>
+    <t>remote.evi</t>
+  </si>
+  <si>
+    <t>Enhanced Vegetation Index (EVI)</t>
+  </si>
+  <si>
+    <t>Index using blue, red, and NIR; reduces background/atmospheric effects.</t>
+  </si>
+  <si>
+    <t>remote.ndvi</t>
+  </si>
+  <si>
+    <t>Normalized Difference Vegetation Index (NDVI)</t>
+  </si>
+  <si>
+    <t>Index for assessing vegetation health from NIR and red reflectance.</t>
+  </si>
+  <si>
+    <t>remote.ndwi</t>
+  </si>
+  <si>
+    <t>Normalized Difference Water Index (NDWI)</t>
+  </si>
+  <si>
+    <t>Index from green and NIR; indicates water presence/moisture.</t>
+  </si>
+  <si>
+    <t>Normalized Difference Chlorophyll Index</t>
+  </si>
+  <si>
+    <t>Maximum Chlorophyll Index</t>
+  </si>
+  <si>
+    <t>Blue Wide Dynamic Range Vegetation Index</t>
+  </si>
+  <si>
+    <t>Enhanced Vegetation Index</t>
+  </si>
+  <si>
+    <t>Normalized Difference Vegetation Index</t>
+  </si>
+  <si>
+    <t>Normalized Difference Water Index</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Normalized Diffrence Chlorophyll Index'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Maximum Chloroprence Chlorophyll Index'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Blue Wide Dynamrence Chlorophyll Index'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Enhanced Vegetarence Chlorophyll Index'</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1245,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1235,11 +1331,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Collegamento ipertestuale 2" xfId="2" xr:uid="{2FCB844D-8848-4EB2-8C88-A6D12B4D0B5A}"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1628,24 +1727,24 @@
   </sheetPr>
   <dimension ref="A1:AZ26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.453125" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="56.58984375" customWidth="1"/>
-    <col min="4" max="4" width="38.76953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.31640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.04296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.58984375" customWidth="1"/>
-    <col min="8" max="8" width="12.58984375" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="56.5546875" customWidth="1"/>
+    <col min="4" max="4" width="38.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -1674,7 +1773,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>104</v>
       </c>
@@ -1700,7 +1799,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:52" s="6" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:52" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>201</v>
       </c>
@@ -1765,7 +1864,7 @@
       <c r="AY3"/>
       <c r="AZ3"/>
     </row>
-    <row r="4" spans="1:52" s="6" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:52" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>208</v>
       </c>
@@ -1830,7 +1929,7 @@
       <c r="AY4"/>
       <c r="AZ4"/>
     </row>
-    <row r="5" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>312</v>
       </c>
@@ -1895,7 +1994,7 @@
       <c r="AY5"/>
       <c r="AZ5"/>
     </row>
-    <row r="6" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>296</v>
       </c>
@@ -1960,7 +2059,7 @@
       <c r="AY6"/>
       <c r="AZ6"/>
     </row>
-    <row r="7" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
@@ -2010,7 +2109,7 @@
       <c r="AY7"/>
       <c r="AZ7"/>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -2021,7 +2120,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2032,7 +2131,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -2043,7 +2142,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2054,7 +2153,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2065,7 +2164,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -2076,7 +2175,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -2087,10 +2186,10 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.75">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C26" s="3"/>
     </row>
   </sheetData>
@@ -2118,16 +2217,16 @@
   <sheetViews>
     <sheetView zoomScale="99" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.6796875" customWidth="1"/>
-    <col min="2" max="2" width="11.58984375" customWidth="1"/>
-    <col min="3" max="3" width="36.26953125" customWidth="1"/>
-    <col min="4" max="4" width="39.6796875" customWidth="1"/>
-    <col min="5" max="5" width="35.1328125" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
@@ -2144,7 +2243,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>107</v>
       </c>
@@ -2161,7 +2260,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>135</v>
       </c>
@@ -2178,7 +2277,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>108</v>
       </c>
@@ -2195,7 +2294,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>109</v>
       </c>
@@ -2212,7 +2311,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>118</v>
       </c>
@@ -2229,7 +2328,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>136</v>
       </c>
@@ -2246,7 +2345,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>114</v>
       </c>
@@ -2263,7 +2362,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>152</v>
       </c>
@@ -2294,19 +2393,19 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.86328125" customWidth="1"/>
-    <col min="3" max="3" width="36.04296875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.2265625" customWidth="1"/>
+    <col min="1" max="1" width="58.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36" style="5" customWidth="1"/>
+    <col min="4" max="4" width="44.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.21875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="11.1328125" customWidth="1"/>
-    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="37.5546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2332,7 +2431,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2359,7 +2458,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2384,7 +2483,7 @@
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2412,7 +2511,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2440,7 +2539,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2465,7 +2564,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2492,7 +2591,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2517,7 +2616,7 @@
       </c>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2540,7 +2639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2565,7 +2664,7 @@
       </c>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2590,7 +2689,7 @@
       </c>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2615,7 +2714,7 @@
       </c>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2640,7 +2739,7 @@
       </c>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2665,7 +2764,7 @@
       </c>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2690,7 +2789,7 @@
       </c>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2715,7 +2814,7 @@
       </c>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2740,7 +2839,7 @@
       </c>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2765,7 +2864,7 @@
       </c>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2790,7 +2889,7 @@
       </c>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2817,7 +2916,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2842,7 +2941,7 @@
       </c>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2867,7 +2966,7 @@
       </c>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2892,7 +2991,7 @@
       </c>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2919,7 +3018,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$6</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/DataSet</v>
@@ -2986,17 +3085,17 @@
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.86328125" customWidth="1"/>
-    <col min="2" max="2" width="11.58984375" customWidth="1"/>
-    <col min="3" max="3" width="15.76953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.6796875" customWidth="1"/>
-    <col min="5" max="5" width="35.1328125" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="53.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -3013,7 +3112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>250</v>
       </c>
@@ -3030,7 +3129,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
         <v>214</v>
       </c>
@@ -3047,7 +3146,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>67</v>
       </c>
@@ -3064,7 +3163,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>219</v>
       </c>
@@ -3081,7 +3180,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>141</v>
       </c>
@@ -3098,7 +3197,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
         <v>253</v>
       </c>
@@ -3115,7 +3214,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>218</v>
       </c>
@@ -3132,7 +3231,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
         <v>212</v>
       </c>
@@ -3149,7 +3248,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>106</v>
       </c>
@@ -3166,7 +3265,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
         <v>275</v>
       </c>
@@ -3183,7 +3282,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="59" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
         <v>272</v>
       </c>
@@ -3200,7 +3299,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="35" t="s">
         <v>213</v>
       </c>
@@ -3217,7 +3316,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="35" t="s">
         <v>228</v>
       </c>
@@ -3234,7 +3333,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>105</v>
       </c>
@@ -3251,7 +3350,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>223</v>
       </c>
@@ -3268,7 +3367,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35" t="s">
         <v>234</v>
       </c>
@@ -3285,7 +3384,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="34" t="s">
         <v>235</v>
       </c>
@@ -3302,7 +3401,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="34" t="s">
         <v>236</v>
       </c>
@@ -3319,7 +3418,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
         <v>237</v>
       </c>
@@ -3336,7 +3435,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
         <v>238</v>
       </c>
@@ -3367,16 +3466,16 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="11.58984375" customWidth="1"/>
-    <col min="3" max="3" width="36.26953125" customWidth="1"/>
-    <col min="4" max="4" width="39.6796875" customWidth="1"/>
-    <col min="5" max="5" width="35.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
@@ -3393,7 +3492,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>122</v>
       </c>
@@ -3410,7 +3509,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>141</v>
       </c>
@@ -3427,7 +3526,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>106</v>
       </c>
@@ -3444,7 +3543,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>151</v>
       </c>
@@ -3461,7 +3560,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>149</v>
       </c>
@@ -3478,7 +3577,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>132</v>
       </c>
@@ -3495,7 +3594,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>145</v>
       </c>
@@ -3512,7 +3611,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>150</v>
       </c>
@@ -3545,15 +3644,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.58984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.31640625" customWidth="1"/>
-    <col min="3" max="3" width="28.04296875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="71.5" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28" style="5" customWidth="1"/>
+    <col min="4" max="4" width="71.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -3567,7 +3666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>100</v>
       </c>
@@ -3581,7 +3680,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>157</v>
       </c>
@@ -3595,7 +3694,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>156</v>
       </c>
@@ -3609,7 +3708,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>123</v>
       </c>
@@ -3623,7 +3722,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>247</v>
       </c>
@@ -3655,23 +3754,25 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.86328125" customWidth="1"/>
-    <col min="3" max="3" width="76.81640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.2265625" customWidth="1"/>
+    <col min="1" max="1" width="58.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.88671875" customWidth="1"/>
+    <col min="3" max="3" width="76.77734375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="44.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.21875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="11.1328125" customWidth="1"/>
-    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="37.5546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3697,7 +3798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -3722,7 +3823,7 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -3752,7 +3853,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -3779,7 +3880,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -3806,7 +3907,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -3833,7 +3934,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -3860,7 +3961,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -3887,7 +3988,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -3912,7 +4013,7 @@
       </c>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -3939,7 +4040,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -3966,7 +4067,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -3993,7 +4094,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4018,7 +4119,7 @@
       </c>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4045,7 +4146,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4072,7 +4173,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4099,7 +4200,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4126,7 +4227,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4153,7 +4254,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4180,7 +4281,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4207,7 +4308,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4234,7 +4335,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4261,7 +4362,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4288,7 +4389,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4313,7 +4414,7 @@
       </c>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4340,7 +4441,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4367,7 +4468,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4394,7 +4495,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4421,7 +4522,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4448,7 +4549,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4475,7 +4576,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4502,14 +4603,149 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.75">
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.75">
-      <c r="C34" s="8"/>
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>343</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4527,20 +4763,22 @@
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0"/>
+    <sheetView topLeftCell="C25" zoomScale="99" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.86328125" customWidth="1"/>
-    <col min="2" max="2" width="11.58984375" customWidth="1"/>
-    <col min="3" max="3" width="36.26953125" customWidth="1"/>
-    <col min="4" max="4" width="39.6796875" customWidth="1"/>
-    <col min="5" max="5" width="35.1328125" customWidth="1"/>
+    <col min="1" max="1" width="53.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
@@ -4557,7 +4795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -4574,7 +4812,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>71</v>
       </c>
@@ -4591,7 +4829,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>72</v>
       </c>
@@ -4608,7 +4846,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>73</v>
       </c>
@@ -4625,7 +4863,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>74</v>
       </c>
@@ -4642,7 +4880,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>75</v>
       </c>
@@ -4659,7 +4897,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>76</v>
       </c>
@@ -4676,7 +4914,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="177" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -4693,7 +4931,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>78</v>
       </c>
@@ -4710,7 +4948,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>79</v>
       </c>
@@ -4727,7 +4965,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>80</v>
       </c>
@@ -4744,7 +4982,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="206.5" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>81</v>
       </c>
@@ -4761,7 +4999,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>82</v>
       </c>
@@ -4778,7 +5016,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>83</v>
       </c>
@@ -4795,7 +5033,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>84</v>
       </c>
@@ -4812,7 +5050,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>85</v>
       </c>
@@ -4829,7 +5067,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>86</v>
       </c>
@@ -4846,7 +5084,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
         <v>87</v>
       </c>
@@ -4863,7 +5101,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>88</v>
       </c>
@@ -4880,7 +5118,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
         <v>89</v>
       </c>
@@ -4897,7 +5135,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
         <v>90</v>
       </c>
@@ -4914,7 +5152,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
         <v>91</v>
       </c>
@@ -4931,7 +5169,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="147.5" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>92</v>
       </c>
@@ -4948,7 +5186,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>93</v>
       </c>
@@ -4965,7 +5203,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>94</v>
       </c>
@@ -4982,7 +5220,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>95</v>
       </c>
@@ -4999,7 +5237,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>96</v>
       </c>
@@ -5016,7 +5254,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
         <v>97</v>
       </c>
@@ -5033,7 +5271,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
         <v>98</v>
       </c>
@@ -5050,7 +5288,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
         <v>99</v>
       </c>
@@ -5065,6 +5303,125 @@
       </c>
       <c r="E31" s="25" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="43" t="s">
+        <v>316</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="22" t="s">
+        <v>318</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>319</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>319</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>319</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>319</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>319</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>319</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -5083,19 +5440,19 @@
       <selection activeCell="G5" sqref="G5:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.86328125" customWidth="1"/>
-    <col min="3" max="3" width="24.76953125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="31.26953125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="31.26953125" customWidth="1"/>
+    <col min="1" max="1" width="58.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="31.21875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="31.21875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="11.1328125" customWidth="1"/>
-    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="37.5546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5121,7 +5478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/SimpleIndicator</v>
@@ -5148,7 +5505,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/SimpleIndicator</v>
@@ -5173,7 +5530,7 @@
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/SimpleIndicator</v>
@@ -5201,7 +5558,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/SimpleIndicator</v>
@@ -5229,7 +5586,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/SimpleIndicator</v>
@@ -5254,7 +5611,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/SimpleIndicator</v>
@@ -5281,7 +5638,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/SimpleIndicator</v>
@@ -5328,16 +5685,16 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.58984375" customWidth="1"/>
-    <col min="3" max="3" width="32.953125" customWidth="1"/>
-    <col min="4" max="4" width="23.36328125" customWidth="1"/>
-    <col min="5" max="5" width="35.1328125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
@@ -5354,7 +5711,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>122</v>
       </c>
@@ -5371,7 +5728,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>141</v>
       </c>
@@ -5388,7 +5745,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>106</v>
       </c>
@@ -5405,7 +5762,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>151</v>
       </c>
@@ -5422,7 +5779,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>149</v>
       </c>
@@ -5455,19 +5812,19 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.86328125" customWidth="1"/>
-    <col min="3" max="3" width="76.81640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.2265625" customWidth="1"/>
+    <col min="1" max="1" width="58.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.88671875" customWidth="1"/>
+    <col min="3" max="3" width="76.77734375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="44.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.21875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="11.1328125" customWidth="1"/>
-    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="37.5546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5493,7 +5850,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
@@ -5520,7 +5877,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
@@ -5545,7 +5902,7 @@
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
@@ -5573,7 +5930,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
@@ -5601,7 +5958,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
@@ -5626,7 +5983,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
@@ -5653,7 +6010,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
@@ -5678,7 +6035,7 @@
       </c>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
@@ -5703,7 +6060,7 @@
       </c>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
@@ -5748,16 +6105,16 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="11.58984375" customWidth="1"/>
-    <col min="3" max="3" width="36.26953125" customWidth="1"/>
-    <col min="4" max="4" width="39.6796875" customWidth="1"/>
-    <col min="5" max="5" width="35.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
@@ -5774,7 +6131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>122</v>
       </c>
@@ -5791,7 +6148,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>141</v>
       </c>
@@ -5808,7 +6165,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>106</v>
       </c>
@@ -5825,7 +6182,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>151</v>
       </c>
@@ -5842,7 +6199,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>132</v>
       </c>
@@ -5859,7 +6216,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>145</v>
       </c>
@@ -5876,7 +6233,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>150</v>
       </c>
@@ -5909,19 +6266,19 @@
       <selection activeCell="B13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.86328125" customWidth="1"/>
-    <col min="3" max="3" width="36.04296875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.2265625" customWidth="1"/>
+    <col min="1" max="1" width="58.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36" style="5" customWidth="1"/>
+    <col min="4" max="4" width="44.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.21875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="11.1328125" customWidth="1"/>
-    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="37.5546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5947,7 +6304,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
@@ -5974,7 +6331,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
@@ -5999,7 +6356,7 @@
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
@@ -6024,7 +6381,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
@@ -6049,7 +6406,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
@@ -6074,7 +6431,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
@@ -6099,7 +6456,7 @@
       </c>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
@@ -6124,7 +6481,7 @@
       </c>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
@@ -6149,7 +6506,7 @@
       </c>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
@@ -6174,7 +6531,7 @@
       </c>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
@@ -6199,7 +6556,7 @@
       </c>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>

</xml_diff>

<commit_message>
Updated mapping Excel to include additional remote sensing indices
</commit_message>
<xml_diff>
--- a/models-src/oah-models-and-maps.xlsx
+++ b/models-src/oah-models-and-maps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\oah\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA00D202-8EFE-49FF-AD16-AA7F05CA57D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB3A22B-9965-472A-AAB3-A17DA41FC5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
   <sheets>
     <sheet name="ConceptMaps" sheetId="17" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="443">
   <si>
     <t>Group Source</t>
   </si>
@@ -1065,34 +1065,322 @@
     <t>Index from green and NIR; indicates water presence/moisture.</t>
   </si>
   <si>
-    <t>Normalized Difference Chlorophyll Index</t>
-  </si>
-  <si>
-    <t>Maximum Chlorophyll Index</t>
-  </si>
-  <si>
-    <t>Blue Wide Dynamic Range Vegetation Index</t>
-  </si>
-  <si>
-    <t>Enhanced Vegetation Index</t>
-  </si>
-  <si>
-    <t>Normalized Difference Vegetation Index</t>
-  </si>
-  <si>
-    <t>Normalized Difference Water Index</t>
-  </si>
-  <si>
-    <t>where Observation.code is 'Normalized Diffrence Chlorophyll Index'</t>
-  </si>
-  <si>
-    <t>where Observation.code is 'Maximum Chloroprence Chlorophyll Index'</t>
-  </si>
-  <si>
-    <t>where Observation.code is 'Blue Wide Dynamrence Chlorophyll Index'</t>
-  </si>
-  <si>
-    <t>where Observation.code is 'Enhanced Vegetarence Chlorophyll Index'</t>
+    <t>remote.mndvi</t>
+  </si>
+  <si>
+    <t>Modified Normalized Difference Vegetation Index (mNDVI)</t>
+  </si>
+  <si>
+    <t>Modified NDVI</t>
+  </si>
+  <si>
+    <t>remote.evi2</t>
+  </si>
+  <si>
+    <t>Enhanced Vegetation Index  2 (EVI2)</t>
+  </si>
+  <si>
+    <t>EVI without the blue band</t>
+  </si>
+  <si>
+    <t>remote.savi</t>
+  </si>
+  <si>
+    <t>remote.tsavi</t>
+  </si>
+  <si>
+    <t>remote.lwci</t>
+  </si>
+  <si>
+    <t>remote.gvmi</t>
+  </si>
+  <si>
+    <t>remote.gemi</t>
+  </si>
+  <si>
+    <t>remote.ndmi</t>
+  </si>
+  <si>
+    <t>remote.lai</t>
+  </si>
+  <si>
+    <t>remote.glai</t>
+  </si>
+  <si>
+    <t>remote.fapar</t>
+  </si>
+  <si>
+    <t>remote.mndwi</t>
+  </si>
+  <si>
+    <t>remote.andwi</t>
+  </si>
+  <si>
+    <t>remote.s2wi</t>
+  </si>
+  <si>
+    <t>remote.lswi</t>
+  </si>
+  <si>
+    <t>remote.ndvi_mndwi_model</t>
+  </si>
+  <si>
+    <t>remote.lst</t>
+  </si>
+  <si>
+    <t>remote.blfei</t>
+  </si>
+  <si>
+    <t>remote.brba</t>
+  </si>
+  <si>
+    <t>remote.nbai</t>
+  </si>
+  <si>
+    <t>remote.ibi</t>
+  </si>
+  <si>
+    <t>remote.ebbi</t>
+  </si>
+  <si>
+    <t>remote.pisi</t>
+  </si>
+  <si>
+    <t>remote.ui</t>
+  </si>
+  <si>
+    <t>remote.vibi</t>
+  </si>
+  <si>
+    <t>Soil Adjusted Vegetation Index (SAVI)</t>
+  </si>
+  <si>
+    <t>Soil-adjusted VI (unitless; needs L factor in method/notes)</t>
+  </si>
+  <si>
+    <t>Transformed SAVI (unitless)</t>
+  </si>
+  <si>
+    <t>Estimates relative leaf water content from spectral bands</t>
+  </si>
+  <si>
+    <t>Detects vegetation water content using NIR and SWIR</t>
+  </si>
+  <si>
+    <t>Global index for vegetation monitoring with reduced atmospheric effects</t>
+  </si>
+  <si>
+    <t>Measures vegetation moisture using NIR and SWIR</t>
+  </si>
+  <si>
+    <t>Leaf surface area per ground area (m²/m²)</t>
+  </si>
+  <si>
+    <t>Green leaf surface area per ground area (m²/m²)</t>
+  </si>
+  <si>
+    <t>Fraction of absorbed photosynthetically active radiation</t>
+  </si>
+  <si>
+    <t>Highlights water features using NIR and Green bands</t>
+  </si>
+  <si>
+    <t>Modified NDWI improving open water detection in urban areas</t>
+  </si>
+  <si>
+    <t>NDWI variant enhancing water body separation</t>
+  </si>
+  <si>
+    <t>Sentinel-2 specific water index</t>
+  </si>
+  <si>
+    <t>Detects water content in vegetation and soil</t>
+  </si>
+  <si>
+    <t>Combined vegetation and water index model</t>
+  </si>
+  <si>
+    <t>Land surface temperature in Kelvin or Celsius</t>
+  </si>
+  <si>
+    <t>Extracts built-up land features from spectral data</t>
+  </si>
+  <si>
+    <t>Band ratio index for built-up area detection</t>
+  </si>
+  <si>
+    <t>Normalized index for built-up area identification</t>
+  </si>
+  <si>
+    <t>Built-up detection using multi-index combination</t>
+  </si>
+  <si>
+    <t>Enhances contrast between built-up and bare areas</t>
+  </si>
+  <si>
+    <t>Measures impervious surface presence</t>
+  </si>
+  <si>
+    <t>Differentiates urban from vegetation areas</t>
+  </si>
+  <si>
+    <t>Combines vegetation and built-up indices for urban analysis</t>
+  </si>
+  <si>
+    <t>Leaf Water Content Index (LWCI)</t>
+  </si>
+  <si>
+    <t>Global Vegetation Moisture Index (GVMI)</t>
+  </si>
+  <si>
+    <t>Global Environment Monitoring Index (GEMI)</t>
+  </si>
+  <si>
+    <t>Normalized Difference Moisture Index (NDMI)</t>
+  </si>
+  <si>
+    <t>Leaf Area Index (LAI)</t>
+  </si>
+  <si>
+    <t>Green Leaf Area Index (GLAI)</t>
+  </si>
+  <si>
+    <t>Fraction of Absorbed Photosynthetically Active Radiation (FAPAR)</t>
+  </si>
+  <si>
+    <t>Modified Normalized Difference Water Index (MNDWI)</t>
+  </si>
+  <si>
+    <t>Augmented Normalized Difference Water Index (ANDWI)</t>
+  </si>
+  <si>
+    <t>Sentinel-2 Water Index (S2WI)</t>
+  </si>
+  <si>
+    <t>Land Surface Water Index (LSWI)</t>
+  </si>
+  <si>
+    <t>NDVI–MNDWI Model</t>
+  </si>
+  <si>
+    <t>Land Surface Temperature (LST)</t>
+  </si>
+  <si>
+    <t>Built-Up Land Features Extraction Index (BLFEI)</t>
+  </si>
+  <si>
+    <t>Band Ratio for Built-up Area (BRBA)</t>
+  </si>
+  <si>
+    <t>Normalized Built-up Area Index (NBAI)</t>
+  </si>
+  <si>
+    <t>Index-Based Built-Up Index (IBI)</t>
+  </si>
+  <si>
+    <t>Enhanced Built-Up and Bareness Index (EBBI)</t>
+  </si>
+  <si>
+    <t>Perpendicular Impervious Surface Index (PISI)</t>
+  </si>
+  <si>
+    <t>Urban Index (UI)</t>
+  </si>
+  <si>
+    <t>Vegetation Index Built-up Index (VIBI)</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Leaf Water Content Index (LWCI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Global Vegetation Moisture Index (GVMI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Global Environment Monitoring Index (GEMI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Normalized Difference Moisture Index (NDMI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Leaf Area Index (LAI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Green Leaf Area Index (GLAI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Fraction of Absorbed Photosynthetically Active Radiation (FAPAR)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Normalized Difference Water Index (NDWI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Modified Normalized Difference Water Index (MNDWI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Augmented Normalized Difference Water Index (ANDWI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Sentinel-2 Water Index (S2WI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Land Surface Water Index (LSWI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'NDVI–MNDWI Model'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Land Surface Temperature (LST)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Built-Up Land Features Extraction Index (BLFEI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Band Ratio for Built-up Area (BRBA)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Normalized Built-up Area Index (NBAI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Index-Based Built-Up Index (IBI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Enhanced Built-Up and Bareness Index (EBBI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Perpendicular Impervious Surface Index (PISI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Urban Index (UI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Vegetation Index Built-up Index (VIBI)'</t>
+  </si>
+  <si>
+    <t>Transformed Soil Adjusted Vegetation Index (TSAVI)</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Transformed Soil Adjusted Vegetation Index (TSAVI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Normalized Difference Chlorophyl Index(NDCI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Blue Wide Dynamic Range Vegetation Index (BWDRVI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Maximum Chlorophyll Index (MCI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Enhanced Vegetation Index (EVI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Normalized Difference Vegetation Index (NDVI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Soil Adjusted Vegetation Index (SAVI)'</t>
+  </si>
+  <si>
+    <t>where Observation.code is 'Enhanced Vegetation Index 2 (EVI2)'</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1533,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1331,9 +1619,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Collegamento ipertestuale 2" xfId="2" xr:uid="{2FCB844D-8848-4EB2-8C88-A6D12B4D0B5A}"/>
@@ -3754,10 +4040,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C34" sqref="A1:H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4615,7 +4901,7 @@
         <v>318</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="E32" s="27" t="s">
         <v>27</v>
@@ -4624,7 +4910,7 @@
         <v>7</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>343</v>
+        <v>436</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4639,7 +4925,7 @@
         <v>322</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="E33" s="27" t="s">
         <v>27</v>
@@ -4648,7 +4934,7 @@
         <v>7</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>344</v>
+        <v>438</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4663,7 +4949,7 @@
         <v>325</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="E34" s="27" t="s">
         <v>27</v>
@@ -4672,7 +4958,7 @@
         <v>7</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>345</v>
+        <v>437</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4687,7 +4973,7 @@
         <v>328</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="E35" s="27" t="s">
         <v>27</v>
@@ -4696,19 +4982,16 @@
         <v>7</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>346</v>
+        <v>439</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
+      <c r="A36" s="7"/>
       <c r="B36" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>341</v>
@@ -4720,7 +5003,7 @@
         <v>7</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>343</v>
+        <v>442</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4732,10 +5015,10 @@
         <v>103</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="E37" s="27" t="s">
         <v>27</v>
@@ -4744,7 +5027,628 @@
         <v>7</v>
       </c>
       <c r="H37" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>343</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E40" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="E43" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="E44" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="E45" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="E46" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="E47" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="E48" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="E50" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="E51" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="E54" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="E55" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="E56" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="E58" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="E59" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="E60" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="E61" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="E62" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="E63" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -4763,10 +5667,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="C25" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="A34" zoomScale="99" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4774,8 +5678,8 @@
     <col min="1" max="1" width="53.88671875" customWidth="1"/>
     <col min="2" max="2" width="11.5546875" customWidth="1"/>
     <col min="3" max="3" width="36.21875" customWidth="1"/>
-    <col min="4" max="4" width="39.6640625" customWidth="1"/>
-    <col min="5" max="5" width="35.109375" customWidth="1"/>
+    <col min="4" max="4" width="50.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -4795,7 +5699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -4812,7 +5716,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>71</v>
       </c>
@@ -4829,7 +5733,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>72</v>
       </c>
@@ -4846,7 +5750,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>73</v>
       </c>
@@ -4863,7 +5767,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>74</v>
       </c>
@@ -4914,7 +5818,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -4931,7 +5835,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>78</v>
       </c>
@@ -4948,7 +5852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>79</v>
       </c>
@@ -4982,7 +5886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>81</v>
       </c>
@@ -4999,7 +5903,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>82</v>
       </c>
@@ -5169,7 +6073,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>92</v>
       </c>
@@ -5186,7 +6090,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>93</v>
       </c>
@@ -5305,31 +6209,31 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
         <v>315</v>
       </c>
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="43" t="s">
+      <c r="D32" t="s">
         <v>316</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="41" t="s">
         <v>319</v>
       </c>
       <c r="D33" s="22" t="s">
@@ -5339,14 +6243,14 @@
         <v>321</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="41" t="s">
         <v>319</v>
       </c>
       <c r="D34" s="22" t="s">
@@ -5356,14 +6260,14 @@
         <v>324</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
         <v>325</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="41" t="s">
         <v>319</v>
       </c>
       <c r="D35" s="22" t="s">
@@ -5373,14 +6277,14 @@
         <v>327</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
         <v>328</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="42" t="s">
+      <c r="C36" s="41" t="s">
         <v>319</v>
       </c>
       <c r="D36" s="22" t="s">
@@ -5390,38 +6294,480 @@
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="22" t="s">
         <v>331</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B38" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C38" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D38" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E38" s="25" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="22" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="22" t="s">
         <v>334</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B40" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C40" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D40" s="22" t="s">
         <v>335</v>
       </c>
-      <c r="E38" s="25" t="s">
+      <c r="E40" s="25" t="s">
         <v>336</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>366</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>434</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>391</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>393</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>394</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>395</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>396</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>397</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="22" t="s">
+        <v>352</v>
+      </c>
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>398</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>399</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>400</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="B55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>402</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="B59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="22" t="s">
+        <v>361</v>
+      </c>
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="B61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="22" t="s">
+        <v>364</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="E63" s="22" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="22" t="s">
+        <v>365</v>
+      </c>
+      <c r="B64" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="D64" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in in models-src/oah-models-and-maps.xlsx
</commit_message>
<xml_diff>
--- a/models-src/oah-models-and-maps.xlsx
+++ b/models-src/oah-models-and-maps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\oah\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB3A22B-9965-472A-AAB3-A17DA41FC5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F6C8D3-2562-4486-8B9C-3522C11730E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="443">
   <si>
     <t>Group Source</t>
   </si>
@@ -1533,7 +1533,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1620,6 +1620,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Collegamento ipertestuale 2" xfId="2" xr:uid="{2FCB844D-8848-4EB2-8C88-A6D12B4D0B5A}"/>
@@ -4040,10 +4047,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C34" sqref="A1:H63"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4263,7 +4270,7 @@
         <f>IndicatorsOah!D8</f>
         <v>Microbiomes/Biofilms</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F8" s="6"/>
@@ -4290,7 +4297,7 @@
         <f>IndicatorsOah!D9</f>
         <v>Key hydromorphological quality indicators</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F9" s="6"/>
@@ -4315,7 +4322,7 @@
         <f>IndicatorsOah!D10</f>
         <v>Morphology of the streams</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="6"/>
@@ -4342,7 +4349,7 @@
         <f>IndicatorsOah!D11</f>
         <v>Hydrology of the stream</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F11" s="6"/>
@@ -4369,7 +4376,7 @@
         <f>IndicatorsOah!D12</f>
         <v>Land use in the margins</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F12" s="6"/>
@@ -4396,7 +4403,7 @@
         <f>IndicatorsOah!D13</f>
         <v>Key water quality indicators</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F13" s="6"/>
@@ -4421,7 +4428,7 @@
         <f>IndicatorsOah!D14</f>
         <v>Nutrients</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F14" s="6"/>
@@ -4448,7 +4455,7 @@
         <f>IndicatorsOah!D15</f>
         <v>pH</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F15" s="6"/>
@@ -4475,7 +4482,7 @@
         <f>IndicatorsOah!D16</f>
         <v>Dissolved O2</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F16" s="6"/>
@@ -4502,7 +4509,7 @@
         <f>IndicatorsOah!D17</f>
         <v>Water temperature</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="6"/>
@@ -4529,7 +4536,7 @@
         <f>IndicatorsOah!D18</f>
         <v>Total dissolved solids (TDS)</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F18" s="6"/>
@@ -4556,7 +4563,7 @@
         <f>IndicatorsOah!D19</f>
         <v>Total suspended solids (TSS)</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F19" s="6"/>
@@ -4583,7 +4590,7 @@
         <f>IndicatorsOah!D20</f>
         <v>Conductivity</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F20" s="6"/>
@@ -4610,7 +4617,7 @@
         <f>IndicatorsOah!D21</f>
         <v>Pharmaceuticals</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F21" s="6"/>
@@ -4637,7 +4644,7 @@
         <f>IndicatorsOah!D22</f>
         <v>Foam/colour/smell</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F22" s="6"/>
@@ -4664,7 +4671,7 @@
         <f>IndicatorsOah!D23</f>
         <v>Coliforms</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F23" s="6"/>
@@ -4691,7 +4698,7 @@
         <f>IndicatorsOah!D24</f>
         <v>Biological indicators of health risks</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F24" s="6"/>
@@ -4716,7 +4723,7 @@
         <f>IndicatorsOah!D25</f>
         <v>Diptera</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F25" s="6"/>
@@ -4743,7 +4750,7 @@
         <f>IndicatorsOah!D26</f>
         <v>Ticks</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F26" s="6"/>
@@ -4770,7 +4777,7 @@
         <f>IndicatorsOah!D27</f>
         <v>Invasive invertebrate, plants and fish</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F27" s="6"/>
@@ -4797,7 +4804,7 @@
         <f>IndicatorsOah!D28</f>
         <v>Birds</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F28" s="6"/>
@@ -4824,7 +4831,7 @@
         <f>IndicatorsOah!D29</f>
         <v>Diatom teratology</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F29" s="6"/>
@@ -4851,7 +4858,7 @@
         <f>IndicatorsOah!D30</f>
         <v>Fish</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="6"/>
@@ -4878,7 +4885,7 @@
         <f>IndicatorsOah!D31</f>
         <v>Amphibians</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="44" t="s">
         <v>27</v>
       </c>
       <c r="F31" s="6"/>
@@ -4889,7 +4896,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -4898,20 +4905,19 @@
         <v>103</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>320</v>
+        <v>315</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>316</v>
       </c>
       <c r="E32" s="27" t="s">
         <v>27</v>
       </c>
+      <c r="F32" s="43"/>
       <c r="G32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="5" t="s">
-        <v>436</v>
-      </c>
+      <c r="H32" s="42"/>
     </row>
     <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="str">
@@ -4922,10 +4928,10 @@
         <v>103</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E33" s="27" t="s">
         <v>27</v>
@@ -4934,7 +4940,7 @@
         <v>7</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4946,10 +4952,10 @@
         <v>103</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E34" s="27" t="s">
         <v>27</v>
@@ -4958,7 +4964,7 @@
         <v>7</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4969,11 +4975,11 @@
       <c r="B35" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>328</v>
+      <c r="C35" s="8" t="s">
+        <v>325</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E35" s="27" t="s">
         <v>27</v>
@@ -4982,19 +4988,22 @@
         <v>7</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+      <c r="A36" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
       <c r="B36" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="E36" s="27" t="s">
         <v>27</v>
@@ -5003,43 +5012,43 @@
         <v>7</v>
       </c>
       <c r="H36" s="5" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="5" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="str">
+    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="E37" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
       <c r="B38" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E38" s="27" t="s">
         <v>27</v>
@@ -5048,22 +5057,19 @@
         <v>7</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
-      </c>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
       <c r="B39" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="E39" s="27" t="s">
         <v>27</v>
@@ -5072,7 +5078,7 @@
         <v>7</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5084,10 +5090,10 @@
         <v>103</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>366</v>
+        <v>335</v>
       </c>
       <c r="E40" s="27" t="s">
         <v>27</v>
@@ -5096,7 +5102,7 @@
         <v>7</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>441</v>
+        <v>419</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5108,10 +5114,10 @@
         <v>103</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>434</v>
+        <v>366</v>
       </c>
       <c r="E41" s="27" t="s">
         <v>27</v>
@@ -5120,7 +5126,7 @@
         <v>7</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5132,10 +5138,10 @@
         <v>103</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="E42" s="27" t="s">
         <v>27</v>
@@ -5144,7 +5150,7 @@
         <v>7</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>412</v>
+        <v>435</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5156,10 +5162,10 @@
         <v>103</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E43" s="27" t="s">
         <v>27</v>
@@ -5168,7 +5174,7 @@
         <v>7</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5180,10 +5186,10 @@
         <v>103</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E44" s="27" t="s">
         <v>27</v>
@@ -5192,7 +5198,7 @@
         <v>7</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5204,10 +5210,10 @@
         <v>103</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E45" s="27" t="s">
         <v>27</v>
@@ -5216,7 +5222,7 @@
         <v>7</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5228,10 +5234,10 @@
         <v>103</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E46" s="27" t="s">
         <v>27</v>
@@ -5240,7 +5246,7 @@
         <v>7</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5252,10 +5258,10 @@
         <v>103</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E47" s="27" t="s">
         <v>27</v>
@@ -5264,10 +5270,10 @@
         <v>7</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -5276,10 +5282,10 @@
         <v>103</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E48" s="27" t="s">
         <v>27</v>
@@ -5288,10 +5294,10 @@
         <v>7</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -5300,10 +5306,10 @@
         <v>103</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>334</v>
+        <v>351</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>335</v>
+        <v>397</v>
       </c>
       <c r="E49" s="27" t="s">
         <v>27</v>
@@ -5312,10 +5318,10 @@
         <v>7</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -5324,10 +5330,10 @@
         <v>103</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>398</v>
+        <v>335</v>
       </c>
       <c r="E50" s="27" t="s">
         <v>27</v>
@@ -5336,7 +5342,7 @@
         <v>7</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -5348,10 +5354,10 @@
         <v>103</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E51" s="27" t="s">
         <v>27</v>
@@ -5360,10 +5366,10 @@
         <v>7</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
@@ -5372,10 +5378,10 @@
         <v>103</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E52" s="27" t="s">
         <v>27</v>
@@ -5384,7 +5390,7 @@
         <v>7</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5396,10 +5402,10 @@
         <v>103</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E53" s="27" t="s">
         <v>27</v>
@@ -5408,7 +5414,7 @@
         <v>7</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5420,10 +5426,10 @@
         <v>103</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E54" s="27" t="s">
         <v>27</v>
@@ -5432,7 +5438,7 @@
         <v>7</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5444,10 +5450,10 @@
         <v>103</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E55" s="27" t="s">
         <v>27</v>
@@ -5456,7 +5462,7 @@
         <v>7</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5468,10 +5474,10 @@
         <v>103</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E56" s="27" t="s">
         <v>27</v>
@@ -5480,7 +5486,7 @@
         <v>7</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5492,10 +5498,10 @@
         <v>103</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E57" s="27" t="s">
         <v>27</v>
@@ -5504,7 +5510,7 @@
         <v>7</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5516,10 +5522,10 @@
         <v>103</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E58" s="27" t="s">
         <v>27</v>
@@ -5528,7 +5534,7 @@
         <v>7</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5540,10 +5546,10 @@
         <v>103</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E59" s="27" t="s">
         <v>27</v>
@@ -5552,7 +5558,7 @@
         <v>7</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5564,10 +5570,10 @@
         <v>103</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E60" s="27" t="s">
         <v>27</v>
@@ -5576,7 +5582,7 @@
         <v>7</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5588,10 +5594,10 @@
         <v>103</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E61" s="27" t="s">
         <v>27</v>
@@ -5600,7 +5606,7 @@
         <v>7</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5612,10 +5618,10 @@
         <v>103</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E62" s="27" t="s">
         <v>27</v>
@@ -5624,7 +5630,7 @@
         <v>7</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5636,10 +5642,10 @@
         <v>103</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E63" s="27" t="s">
         <v>27</v>
@@ -5648,6 +5654,30 @@
         <v>7</v>
       </c>
       <c r="H63" s="5" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$2</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/IndicatorsOah</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="E64" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H64" s="5" t="s">
         <v>433</v>
       </c>
     </row>
@@ -5669,8 +5699,8 @@
   </sheetPr>
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="A19" zoomScale="99" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add Health Indicators and Measures models, mappings, and configurations - Introduced new logical models for Health Indicators and Health Measures. - Defined profiles for health measures and observation health measures.
</commit_message>
<xml_diff>
--- a/models-src/oah-models-and-maps.xlsx
+++ b/models-src/oah-models-and-maps.xlsx
@@ -1,37 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\oah\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0BBC34-64D6-423B-93DE-F5A736FB7282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77FB2D5-D379-46D7-A3F6-8BA95B1896C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
   <sheets>
     <sheet name="ConceptMaps" sheetId="17" r:id="rId1"/>
     <sheet name="LogicalModels" sheetId="15" r:id="rId2"/>
-    <sheet name="IndicatorsOah2FHIR" sheetId="54" r:id="rId3"/>
-    <sheet name="IndicatorsOah" sheetId="47" r:id="rId4"/>
-    <sheet name="SimpleIndicatorOah2FHIR" sheetId="34" r:id="rId5"/>
-    <sheet name="SimpleIndicatorOah" sheetId="51" r:id="rId6"/>
-    <sheet name="StructuredIndicatorOah2FHIR" sheetId="55" r:id="rId7"/>
-    <sheet name="StructuredIndicatorOah" sheetId="52" r:id="rId8"/>
-    <sheet name="SampleOah2FHIR" sheetId="57" r:id="rId9"/>
-    <sheet name="SampleOah" sheetId="49" r:id="rId10"/>
-    <sheet name="DataSetOah2FHIR" sheetId="58" r:id="rId11"/>
-    <sheet name="DataSetOah" sheetId="56" r:id="rId12"/>
-    <sheet name="IndicatorOah-notUsed" sheetId="50" r:id="rId13"/>
+    <sheet name="HealthIndicatorsOah2FHIR" sheetId="59" r:id="rId3"/>
+    <sheet name="HealthIndicatorsOah" sheetId="60" r:id="rId4"/>
+    <sheet name="IndicatorsOah2FHIR" sheetId="54" r:id="rId5"/>
+    <sheet name="IndicatorsOah" sheetId="47" r:id="rId6"/>
+    <sheet name="HealthMeasureOah2FHIR" sheetId="61" r:id="rId7"/>
+    <sheet name="HealthMeasureOah" sheetId="62" r:id="rId8"/>
+    <sheet name="SimpleIndicatorOah2FHIR" sheetId="34" r:id="rId9"/>
+    <sheet name="SimpleIndicatorOah" sheetId="51" r:id="rId10"/>
+    <sheet name="StructuredIndicatorOah2FHIR" sheetId="55" r:id="rId11"/>
+    <sheet name="StructuredIndicatorOah" sheetId="52" r:id="rId12"/>
+    <sheet name="SampleOah2FHIR" sheetId="57" r:id="rId13"/>
+    <sheet name="SampleOah" sheetId="49" r:id="rId14"/>
+    <sheet name="DataSetOah2FHIR" sheetId="58" r:id="rId15"/>
+    <sheet name="DataSetOah" sheetId="56" r:id="rId16"/>
+    <sheet name="IndicatorOah-notUsed" sheetId="50" r:id="rId17"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId14"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">DataSetOah!$A$1:$E$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">DataSetOah!$A$1:$E$9</definedName>
     <definedName name="CENEN13606Lekarska_prepustacia_sprava">'[1]Hospital Discharge Report '!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -52,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="493">
   <si>
     <t>Group Source</t>
   </si>
@@ -1276,13 +1280,268 @@
   </si>
   <si>
     <t>remote.ndviMndwiModel</t>
+  </si>
+  <si>
+    <t>diseasePrevalence</t>
+  </si>
+  <si>
+    <t>% of people with long-term disease</t>
+  </si>
+  <si>
+    <t>% of people without  long-term disease</t>
+  </si>
+  <si>
+    <t>% of people with BMI &lt;18,5</t>
+  </si>
+  <si>
+    <t>% of people with BMI 18,5-24,9</t>
+  </si>
+  <si>
+    <t>% of people with BMI 25-29,9</t>
+  </si>
+  <si>
+    <t>% of people with BMI =&gt;30</t>
+  </si>
+  <si>
+    <t>% of people that have or have had Diabetes, COPD or Cardiovascular disease</t>
+  </si>
+  <si>
+    <t>% of people that do not have Diabetes, COPD or Cardiovascular disease</t>
+  </si>
+  <si>
+    <t>% of people experience with mental health issues</t>
+  </si>
+  <si>
+    <t>% of people with Borrelia Burgdoferi</t>
+  </si>
+  <si>
+    <t>% of people with Campylobacter</t>
+  </si>
+  <si>
+    <t>% of people with Chlamydia Psittaci</t>
+  </si>
+  <si>
+    <t>% of people with Cryptosporidium</t>
+  </si>
+  <si>
+    <t>% of people with Entamoeba histolytica</t>
+  </si>
+  <si>
+    <t>% of people with Escherichia Coli</t>
+  </si>
+  <si>
+    <t>% of people with Giarda</t>
+  </si>
+  <si>
+    <t>% of people with Salmonella</t>
+  </si>
+  <si>
+    <t>% of people with Yersinia enterocolitica</t>
+  </si>
+  <si>
+    <t>% of people with Cases of Gastrointestinal diseases</t>
+  </si>
+  <si>
+    <t>% of people with high blood pressure (prevalence)</t>
+  </si>
+  <si>
+    <t>% of people under treatment for hypertension</t>
+  </si>
+  <si>
+    <t>% of people under treatment for high blood pressure</t>
+  </si>
+  <si>
+    <t>% of people affected from obesity</t>
+  </si>
+  <si>
+    <t>% of people under treatment for hypercholesterolemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of people with high blood sugar/diabetes </t>
+  </si>
+  <si>
+    <t>% of people under treatment for diabetes</t>
+  </si>
+  <si>
+    <t>% of people not engaging in physical activity</t>
+  </si>
+  <si>
+    <t>% of people affected from CVD</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.highBloodPression</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.hypertension</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.highBloodPressionTreatment</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.obesity</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.cholesterolemia190</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.hypercholesterolemiaTreatment</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.cholesterolemia240</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.diabetes</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.diabetesTreatment</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.noPhysicalActivity</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.cvd</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.gastrointestinal</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.longTermDisease</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.noLongTermDisease</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.bmiBelow18</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.bmiBelow25</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.bmiBelow30</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.bmiAbove30</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.diabateCopdCvd</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.noDiabateCopdCvd</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.mentalHealth</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.borrelia</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.campylobacter</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.chlamydia</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.cryptosporidium</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.entamoeba</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.escherichiaColi</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.giarda</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.salmonella</t>
+  </si>
+  <si>
+    <t>diseasePrevalence.yersiniaEnterocolitica</t>
+  </si>
+  <si>
+    <t>HealthIndicatorsOah</t>
+  </si>
+  <si>
+    <t>HealthIndicators</t>
+  </si>
+  <si>
+    <t>Health Indicators</t>
+  </si>
+  <si>
+    <t>Set of OneAquaHealth Health and Wellness indicators</t>
+  </si>
+  <si>
+    <t>HealthIndicatorsOah2FHIR</t>
+  </si>
+  <si>
+    <t>Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</t>
+  </si>
+  <si>
+    <t>Cases of disease prevalence</t>
+  </si>
+  <si>
+    <t>dateOrPeriod[x]</t>
+  </si>
+  <si>
+    <t>dateTime or Period</t>
+  </si>
+  <si>
+    <t>Measure Date or Period</t>
+  </si>
+  <si>
+    <t>Type of indicator : e.g. % of people with Giarda</t>
+  </si>
+  <si>
+    <t>cohort</t>
+  </si>
+  <si>
+    <t>Cohort</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Group of people who share a common characteristic.</t>
+  </si>
+  <si>
+    <t>Observation.effective[x]</t>
+  </si>
+  <si>
+    <t>Observation.focus</t>
+  </si>
+  <si>
+    <t>HealthMeasureOah</t>
+  </si>
+  <si>
+    <t>HealthMeasure</t>
+  </si>
+  <si>
+    <t>Health measure</t>
+  </si>
+  <si>
+    <t>Model describing the common attributes of a simple health and wellness indicator</t>
+  </si>
+  <si>
+    <t>HealthMeasureOah2FHIR</t>
+  </si>
+  <si>
+    <t>% of people with high total cholesterolemia (&gt;=190 mg/dl)</t>
+  </si>
+  <si>
+    <t>% of people with high total cholesterolemia (&gt;=240 mg/dl)</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/ig/oah/StructureDefinition/observation-health-measure-oah</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/ig/oah/StructureDefinition/group-oah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1327,8 +1586,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1371,8 +1643,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1419,6 +1697,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1428,7 +1719,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1517,6 +1808,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1912,7 +2225,7 @@
   <dimension ref="A1:AZ26"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1965,7 +2278,7 @@
         <v>104</v>
       </c>
       <c r="C2" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/ConceptMap/"&amp;A2</f>
+        <f t="shared" ref="C2:C8" si="0">"http://hl7.eu/fhir/ig/oah/ConceptMap/"&amp;A2</f>
         <v>http://hl7.eu/fhir/ig/oah/ConceptMap/IndicatorsOah2FHIR</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -1991,7 +2304,7 @@
         <v>201</v>
       </c>
       <c r="C3" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/ConceptMap/"&amp;A3</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.eu/fhir/ig/oah/ConceptMap/SimpleIndicatorOah2FHIR</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -2056,7 +2369,7 @@
         <v>208</v>
       </c>
       <c r="C4" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/ConceptMap/"&amp;A4</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.eu/fhir/ig/oah/ConceptMap/StructuredIndicatorOah2FHIR</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -2121,7 +2434,7 @@
         <v>312</v>
       </c>
       <c r="C5" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/ConceptMap/"&amp;A5</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.eu/fhir/ig/oah/ConceptMap/SampleOah2FHIR</v>
       </c>
       <c r="D5" s="8" t="s">
@@ -2186,7 +2499,7 @@
         <v>296</v>
       </c>
       <c r="C6" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/ConceptMap/"&amp;A6</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.eu/fhir/ig/oah/ConceptMap/DataSetOah2FHIR</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -2244,10 +2557,25 @@
       <c r="AZ6"/>
     </row>
     <row r="7" spans="1:52" s="6" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="C7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.eu/fhir/ig/oah/ConceptMap/HealthIndicatorsOah2FHIR</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="H7" s="10"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -2294,12 +2622,25 @@
       <c r="AZ7"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.75">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="C8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.eu/fhir/ig/oah/ConceptMap/HealthMeasureOah2FHIR</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" s="6"/>
       <c r="H8" s="10"/>
       <c r="I8" s="6"/>
@@ -2386,20 +2727,942 @@
     <hyperlink ref="C6" r:id="rId4" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{BF0DB1E2-0F2B-4E3E-805E-1CE18721AADF}"/>
     <hyperlink ref="B6" location="DataSetOah2FHIR!A1" display="DataSetOah2FHIR" xr:uid="{269D91BA-A142-452C-BFC2-03E878D7FE34}"/>
     <hyperlink ref="C5" r:id="rId5" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{98932B28-070D-49A9-BFC9-E1569CC7F58A}"/>
+    <hyperlink ref="C7" r:id="rId6" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{B424B8D1-7E93-478C-A503-60C861B1E6A1}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{FD1B42E1-3580-4F05-A2FA-F7B592BC9C46}"/>
+    <hyperlink ref="B8" location="HealthMeasureOah2FHIR!A1" display="#HealthMeasureOah2FHIR!A1" xr:uid="{44EE0C0A-E791-40A6-8F5A-DFE8DF9E21F0}"/>
+    <hyperlink ref="C8" r:id="rId8" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{E27C1DCD-2D51-4829-9A3E-AFCC4D888638}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8917C38-1E9C-4CA8-B026-1EC7F0AF7FE1}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="23.31640625" customWidth="1"/>
+    <col min="5" max="5" width="35.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A6" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A9AEBD-A9A0-493E-863C-D52F8723986B}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="58.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.86328125" customWidth="1"/>
+    <col min="3" max="3" width="76.76953125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.2265625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A2" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="8" t="str">
+        <f>StructuredIndicatorOah!A2</f>
+        <v>sampleDetails</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>StructuredIndicatorOah!D2</f>
+        <v>Sample</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A3" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="8" t="str">
+        <f>StructuredIndicatorOah!A2</f>
+        <v>sampleDetails</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>StructuredIndicatorOah!D2</f>
+        <v>Sample</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A4" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="8" t="str">
+        <f>StructuredIndicatorOah!A2</f>
+        <v>sampleDetails</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f>StructuredIndicatorOah!D2</f>
+        <v>Sample</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="6" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A5" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="8" t="str">
+        <f>StructuredIndicatorOah!A3</f>
+        <v>type</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f>StructuredIndicatorOah!D3</f>
+        <v>What is measured</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" s="6" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A6" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="8" t="str">
+        <f>StructuredIndicatorOah!A4</f>
+        <v>date</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f>StructuredIndicatorOah!D4</f>
+        <v>Observation date</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A7" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>StructuredIndicatorOah!A5</f>
+        <v>performer[x]</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f>StructuredIndicatorOah!D5</f>
+        <v>Who made the measure</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A8" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="8" t="str">
+        <f>StructuredIndicatorOah!A6</f>
+        <v>component</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>StructuredIndicatorOah!D6</f>
+        <v>Component</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A9" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>StructuredIndicatorOah!A7</f>
+        <v>component.type</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>StructuredIndicatorOah!D7</f>
+        <v>What is measured</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A10" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="8" t="str">
+        <f>StructuredIndicatorOah!A8</f>
+        <v>component.result[x]</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>StructuredIndicatorOah!D8</f>
+        <v>Result</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H10" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{0FD19491-9321-40B7-B0F0-8DD001375ACD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8B5A90-6D36-45B7-9347-AA4594F3DFDD}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="3" max="3" width="36.2265625" customWidth="1"/>
+    <col min="4" max="4" width="39.6796875" customWidth="1"/>
+    <col min="5" max="5" width="35.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A6" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A7" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A8" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CAA406-B92E-4F33-947E-7872EDD03684}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="58.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.86328125" customWidth="1"/>
+    <col min="3" max="3" width="36" style="5" customWidth="1"/>
+    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.2265625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A2" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="C2" s="8" t="str">
+        <f>SampleOah!A2</f>
+        <v>site</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>SampleOah!D2</f>
+        <v>Sampling Site</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A3" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="8" t="str">
+        <f>SampleOah!A2</f>
+        <v>site</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>SampleOah!D2</f>
+        <v>Sampling Site</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A4" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4" s="27" t="str">
+        <f>SampleOah!A6</f>
+        <v>site.characteristics</v>
+      </c>
+      <c r="D4" s="27" t="str">
+        <f>SampleOah!D6</f>
+        <v>Characteristics</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A5" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="C5" s="8" t="str">
+        <f>SampleOah!A8</f>
+        <v>dateOfSampling</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f>SampleOah!D8</f>
+        <v>Date of Sample</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A6" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="C6" s="8" t="str">
+        <f>SampleOah!A9</f>
+        <v>perfomer[x]</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f>SampleOah!D9</f>
+        <v>Performer</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A7" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
+      </c>
+      <c r="B7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>SampleOah!A2</f>
+        <v>site</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f>SampleOah!D2</f>
+        <v>Sampling Site</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A8" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
+      </c>
+      <c r="B8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C8" s="8" t="str">
+        <f>SampleOah!A3</f>
+        <v>site.identifier</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>SampleOah!D3</f>
+        <v>Site identifier</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A9" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
+      </c>
+      <c r="B9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>SampleOah!A4</f>
+        <v>site.name</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>SampleOah!D4</f>
+        <v>Site Name</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A10" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
+      </c>
+      <c r="B10" t="s">
+        <v>300</v>
+      </c>
+      <c r="C10" s="8" t="str">
+        <f>SampleOah!A5</f>
+        <v>site.gps</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>SampleOah!D5</f>
+        <v>GPS</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A11" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
+      </c>
+      <c r="B11" t="s">
+        <v>300</v>
+      </c>
+      <c r="C11" s="27" t="str">
+        <f>SampleOah!A6</f>
+        <v>site.characteristics</v>
+      </c>
+      <c r="D11" s="27" t="str">
+        <f>SampleOah!D6</f>
+        <v>Characteristics</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A12" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
+      </c>
+      <c r="B12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C12" s="8" t="str">
+        <f>SampleOah!A7</f>
+        <v>site.formReference</v>
+      </c>
+      <c r="D12" s="8" t="str">
+        <f>SampleOah!D7</f>
+        <v>Form Reference</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H12" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{E181CF34-81EF-44E5-98B8-1A9E617A5F12}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E1E018-F3BA-4B95-9856-259080B6D3DC}">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0"/>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -2568,14 +3831,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1865734-ACDE-47B2-B42F-1DEF5E63BE43}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -3258,7 +4521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31B2C70-17A7-40F9-AE47-E4872DBEC665}">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
@@ -3642,7 +4905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ED8D9E-4C8F-4866-AD65-D95CCFA6E5A0}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -3822,10 +5085,10 @@
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3920,6 +5183,34 @@
         <v>249</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A7" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A8" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>487</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" location="IndicatorsOah!A1" display="IndicatorsOah" xr:uid="{E21EEA15-0E90-4596-8BD9-8A69DCDCC058}"/>
@@ -3927,21 +5218,1528 @@
     <hyperlink ref="B4" location="StructuredIndicatorOah!A1" display="StructuredIndicatorOah" xr:uid="{4BCC05B1-2BDB-4C95-8C70-193FBCF8F983}"/>
     <hyperlink ref="B3" location="SimpleIndicatorOah!A1" display="SimpleIndicatorOah" xr:uid="{1BBB742F-F9D6-4621-914C-BE1DD198CC91}"/>
     <hyperlink ref="B6" location="DataSetOah!A1" display="DataSetOah" xr:uid="{745C93EF-7CD1-4EDC-86A1-68DED4068876}"/>
+    <hyperlink ref="B7" location="HealthIndicatorsOah!A1" display="#HealthIndicatorsOah!A1" xr:uid="{C11E51ED-B0B7-4E81-8F51-6FA7790E9B32}"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{DDC97B00-68EF-4C9B-A4D9-DFFCB86F27E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BACF5BE3-3DB4-4D21-9F67-6450BA65E2E4}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="58.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.86328125" customWidth="1"/>
+    <col min="3" max="3" width="59.1328125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.2265625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A2" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C2" s="8" t="str">
+        <f>HealthIndicatorsOah!A2</f>
+        <v>diseasePrevalence</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>HealthIndicatorsOah!D2</f>
+        <v>Cases of disease prevalence</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A3" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C3" s="8" t="str">
+        <f>HealthIndicatorsOah!A3</f>
+        <v>diseasePrevalence.highBloodPression</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>HealthIndicatorsOah!D3</f>
+        <v>% of people with high blood pressure (prevalence)</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="6" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A4" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C4" s="8" t="str">
+        <f>HealthIndicatorsOah!A4</f>
+        <v>diseasePrevalence.hypertension</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f>HealthIndicatorsOah!D4</f>
+        <v>% of people under treatment for hypertension</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A5" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C5" s="8" t="str">
+        <f>HealthIndicatorsOah!A5</f>
+        <v>diseasePrevalence.highBloodPressionTreatment</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f>HealthIndicatorsOah!D5</f>
+        <v>% of people under treatment for high blood pressure</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A6" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C6" s="8" t="str">
+        <f>HealthIndicatorsOah!A6</f>
+        <v>diseasePrevalence.obesity</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f>HealthIndicatorsOah!D6</f>
+        <v>% of people affected from obesity</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="A7" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>HealthIndicatorsOah!A7</f>
+        <v>diseasePrevalence.cholesterolemia190</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f>HealthIndicatorsOah!D7</f>
+        <v>% of people with high total cholesterolemia (&gt;=190 mg/dl)</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A8" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C8" s="8" t="str">
+        <f>HealthIndicatorsOah!A8</f>
+        <v>diseasePrevalence.hypercholesterolemiaTreatment</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>HealthIndicatorsOah!D8</f>
+        <v>% of people under treatment for hypercholesterolemia</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A9" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>HealthIndicatorsOah!A9</f>
+        <v>diseasePrevalence.cholesterolemia240</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>HealthIndicatorsOah!D9</f>
+        <v>% of people with high total cholesterolemia (&gt;=240 mg/dl)</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A10" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C10" s="8" t="str">
+        <f>HealthIndicatorsOah!A10</f>
+        <v>diseasePrevalence.diabetes</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>HealthIndicatorsOah!D10</f>
+        <v xml:space="preserve">% of people with high blood sugar/diabetes </v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A11" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C11" s="8" t="str">
+        <f>HealthIndicatorsOah!A11</f>
+        <v>diseasePrevalence.diabetesTreatment</v>
+      </c>
+      <c r="D11" s="8" t="str">
+        <f>HealthIndicatorsOah!D11</f>
+        <v>% of people under treatment for diabetes</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A12" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C12" s="8" t="str">
+        <f>HealthIndicatorsOah!A12</f>
+        <v>diseasePrevalence.noPhysicalActivity</v>
+      </c>
+      <c r="D12" s="8" t="str">
+        <f>HealthIndicatorsOah!D12</f>
+        <v>% of people not engaging in physical activity</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A13" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C13" s="8" t="str">
+        <f>HealthIndicatorsOah!A13</f>
+        <v>diseasePrevalence.cvd</v>
+      </c>
+      <c r="D13" s="8" t="str">
+        <f>HealthIndicatorsOah!D13</f>
+        <v>% of people affected from CVD</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A14" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C14" s="8" t="str">
+        <f>HealthIndicatorsOah!A14</f>
+        <v>diseasePrevalence.gastrointestinal</v>
+      </c>
+      <c r="D14" s="8" t="str">
+        <f>HealthIndicatorsOah!D14</f>
+        <v>% of people with Cases of Gastrointestinal diseases</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A15" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C15" s="8" t="str">
+        <f>HealthIndicatorsOah!A15</f>
+        <v>diseasePrevalence.longTermDisease</v>
+      </c>
+      <c r="D15" s="8" t="str">
+        <f>HealthIndicatorsOah!D15</f>
+        <v>% of people with long-term disease</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A16" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C16" s="8" t="str">
+        <f>HealthIndicatorsOah!A16</f>
+        <v>diseasePrevalence.noLongTermDisease</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <f>HealthIndicatorsOah!D16</f>
+        <v>% of people without  long-term disease</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A17" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C17" s="8" t="str">
+        <f>HealthIndicatorsOah!A17</f>
+        <v>diseasePrevalence.bmiBelow18</v>
+      </c>
+      <c r="D17" s="8" t="str">
+        <f>HealthIndicatorsOah!D17</f>
+        <v>% of people with BMI &lt;18,5</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A18" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C18" s="8" t="str">
+        <f>HealthIndicatorsOah!A18</f>
+        <v>diseasePrevalence.bmiBelow25</v>
+      </c>
+      <c r="D18" s="8" t="str">
+        <f>HealthIndicatorsOah!D18</f>
+        <v>% of people with BMI 18,5-24,9</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A19" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C19" s="8" t="str">
+        <f>HealthIndicatorsOah!A19</f>
+        <v>diseasePrevalence.bmiBelow30</v>
+      </c>
+      <c r="D19" s="8" t="str">
+        <f>HealthIndicatorsOah!D19</f>
+        <v>% of people with BMI 25-29,9</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A20" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C20" s="8" t="str">
+        <f>HealthIndicatorsOah!A20</f>
+        <v>diseasePrevalence.bmiAbove30</v>
+      </c>
+      <c r="D20" s="8" t="str">
+        <f>HealthIndicatorsOah!D20</f>
+        <v>% of people with BMI =&gt;30</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A21" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C21" s="8" t="str">
+        <f>HealthIndicatorsOah!A21</f>
+        <v>diseasePrevalence.diabateCopdCvd</v>
+      </c>
+      <c r="D21" s="8" t="str">
+        <f>HealthIndicatorsOah!D21</f>
+        <v>% of people that have or have had Diabetes, COPD or Cardiovascular disease</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A22" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C22" s="8" t="str">
+        <f>HealthIndicatorsOah!A22</f>
+        <v>diseasePrevalence.noDiabateCopdCvd</v>
+      </c>
+      <c r="D22" s="8" t="str">
+        <f>HealthIndicatorsOah!D22</f>
+        <v>% of people that do not have Diabetes, COPD or Cardiovascular disease</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A23" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C23" s="8" t="str">
+        <f>HealthIndicatorsOah!A23</f>
+        <v>diseasePrevalence.mentalHealth</v>
+      </c>
+      <c r="D23" s="8" t="str">
+        <f>HealthIndicatorsOah!D23</f>
+        <v>% of people experience with mental health issues</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A24" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C24" s="8" t="str">
+        <f>HealthIndicatorsOah!A24</f>
+        <v>diseasePrevalence.borrelia</v>
+      </c>
+      <c r="D24" s="8" t="str">
+        <f>HealthIndicatorsOah!D24</f>
+        <v>% of people with Borrelia Burgdoferi</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A25" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C25" s="8" t="str">
+        <f>HealthIndicatorsOah!A25</f>
+        <v>diseasePrevalence.campylobacter</v>
+      </c>
+      <c r="D25" s="8" t="str">
+        <f>HealthIndicatorsOah!D25</f>
+        <v>% of people with Campylobacter</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A26" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C26" s="8" t="str">
+        <f>HealthIndicatorsOah!A26</f>
+        <v>diseasePrevalence.chlamydia</v>
+      </c>
+      <c r="D26" s="8" t="str">
+        <f>HealthIndicatorsOah!D26</f>
+        <v>% of people with Chlamydia Psittaci</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A27" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C27" s="8" t="str">
+        <f>HealthIndicatorsOah!A27</f>
+        <v>diseasePrevalence.cryptosporidium</v>
+      </c>
+      <c r="D27" s="8" t="str">
+        <f>HealthIndicatorsOah!D27</f>
+        <v>% of people with Cryptosporidium</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A28" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C28" s="8" t="str">
+        <f>HealthIndicatorsOah!A28</f>
+        <v>diseasePrevalence.entamoeba</v>
+      </c>
+      <c r="D28" s="8" t="str">
+        <f>HealthIndicatorsOah!D28</f>
+        <v>% of people with Entamoeba histolytica</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A29" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C29" s="8" t="str">
+        <f>HealthIndicatorsOah!A29</f>
+        <v>diseasePrevalence.escherichiaColi</v>
+      </c>
+      <c r="D29" s="8" t="str">
+        <f>HealthIndicatorsOah!D29</f>
+        <v>% of people with Escherichia Coli</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A30" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C30" s="8" t="str">
+        <f>HealthIndicatorsOah!A30</f>
+        <v>diseasePrevalence.giarda</v>
+      </c>
+      <c r="D30" s="8" t="str">
+        <f>HealthIndicatorsOah!D30</f>
+        <v>% of people with Giarda</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A31" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C31" s="8" t="str">
+        <f>HealthIndicatorsOah!A31</f>
+        <v>diseasePrevalence.salmonella</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f>HealthIndicatorsOah!D31</f>
+        <v>% of people with Salmonella</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A32" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$7</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthIndicators</v>
+      </c>
+      <c r="B32" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C32" s="8" t="str">
+        <f>HealthIndicatorsOah!A32</f>
+        <v>diseasePrevalence.yersiniaEnterocolitica</v>
+      </c>
+      <c r="D32" s="8" t="str">
+        <f>HealthIndicatorsOah!D32</f>
+        <v>% of people with Yersinia enterocolitica</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{7ECBB079-59D4-430D-A63D-DA6562D0849D}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{90723054-B35E-4066-95F6-D6C3AEAB7AC6}"/>
+    <hyperlink ref="B3:B32" r:id="rId3" display="http://hl7.eu/fhir/ig/oah/StructureDefinition/observation-health-measure-oah" xr:uid="{71C462B5-7360-4020-99CD-1D62E47FDF48}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1B117A-C1FF-4740-AEDC-306C783F299A}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="53.86328125" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="3" max="3" width="36.2265625" customWidth="1"/>
+    <col min="4" max="4" width="50.2265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="93.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="32" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>473</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A3" s="26" t="s">
+        <v>437</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>428</v>
+      </c>
+      <c r="E3" s="43" t="str">
+        <f>D3&amp;" - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project"</f>
+        <v>% of people with high blood pressure (prevalence) - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+      <c r="L3" s="43"/>
+    </row>
+    <row r="4" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A4" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>429</v>
+      </c>
+      <c r="E4" s="43" t="str">
+        <f t="shared" ref="E4:E32" si="0">D4&amp;" - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project"</f>
+        <v>% of people under treatment for hypertension - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+      <c r="L4" s="43"/>
+    </row>
+    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A5" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>430</v>
+      </c>
+      <c r="E5" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people under treatment for high blood pressure - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="L5" s="43"/>
+    </row>
+    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A6" s="26" t="s">
+        <v>440</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="E6" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people affected from obesity - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+      <c r="L6" s="43"/>
+    </row>
+    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A7" s="32" t="s">
+        <v>441</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>489</v>
+      </c>
+      <c r="E7" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with high total cholesterolemia (&gt;=190 mg/dl) - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+      <c r="L7" s="43"/>
+    </row>
+    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A8" s="33" t="s">
+        <v>442</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>432</v>
+      </c>
+      <c r="E8" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people under treatment for hypercholesterolemia - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+      <c r="L8" s="43"/>
+    </row>
+    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A9" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>490</v>
+      </c>
+      <c r="E9" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with high total cholesterolemia (&gt;=240 mg/dl) - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+      <c r="L9" s="43"/>
+    </row>
+    <row r="10" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A10" s="26" t="s">
+        <v>444</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>433</v>
+      </c>
+      <c r="E10" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with high blood sugar/diabetes  - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+      <c r="L10" s="43"/>
+    </row>
+    <row r="11" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A11" s="26" t="s">
+        <v>445</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>434</v>
+      </c>
+      <c r="E11" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people under treatment for diabetes - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+      <c r="L11" s="43"/>
+    </row>
+    <row r="12" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A12" s="26" t="s">
+        <v>446</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>435</v>
+      </c>
+      <c r="E12" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people not engaging in physical activity - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+      <c r="L12" s="43"/>
+    </row>
+    <row r="13" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A13" s="26" t="s">
+        <v>447</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>436</v>
+      </c>
+      <c r="E13" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people affected from CVD - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+      <c r="L13" s="43"/>
+    </row>
+    <row r="14" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A14" s="26" t="s">
+        <v>448</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>427</v>
+      </c>
+      <c r="E14" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with Cases of Gastrointestinal diseases - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A15" s="26" t="s">
+        <v>449</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>409</v>
+      </c>
+      <c r="E15" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with long-term disease - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="48" x14ac:dyDescent="0.75">
+      <c r="A16" s="26" t="s">
+        <v>450</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>410</v>
+      </c>
+      <c r="E16" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people without  long-term disease - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A17" s="26" t="s">
+        <v>451</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="E17" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with BMI &lt;18,5 - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A18" s="26" t="s">
+        <v>452</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>412</v>
+      </c>
+      <c r="E18" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with BMI 18,5-24,9 - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A19" s="26" t="s">
+        <v>453</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>413</v>
+      </c>
+      <c r="E19" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with BMI 25-29,9 - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A20" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>414</v>
+      </c>
+      <c r="E20" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with BMI =&gt;30 - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="64" x14ac:dyDescent="0.75">
+      <c r="A21" s="49" t="s">
+        <v>455</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>415</v>
+      </c>
+      <c r="E21" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people that have or have had Diabetes, COPD or Cardiovascular disease - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="64" x14ac:dyDescent="0.75">
+      <c r="A22" s="49" t="s">
+        <v>456</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="45" t="s">
+        <v>416</v>
+      </c>
+      <c r="E22" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people that do not have Diabetes, COPD or Cardiovascular disease - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A23" s="49" t="s">
+        <v>457</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="45" t="s">
+        <v>417</v>
+      </c>
+      <c r="E23" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people experience with mental health issues - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A24" s="49" t="s">
+        <v>458</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>418</v>
+      </c>
+      <c r="E24" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with Borrelia Burgdoferi - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A25" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>419</v>
+      </c>
+      <c r="E25" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with Campylobacter - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A26" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>420</v>
+      </c>
+      <c r="E26" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with Chlamydia Psittaci - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A27" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="46" t="s">
+        <v>421</v>
+      </c>
+      <c r="E27" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with Cryptosporidium - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A28" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>422</v>
+      </c>
+      <c r="E28" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with Entamoeba histolytica - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A29" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="46" t="s">
+        <v>423</v>
+      </c>
+      <c r="E29" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with Escherichia Coli - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A30" s="33" t="s">
+        <v>464</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="46" t="s">
+        <v>424</v>
+      </c>
+      <c r="E30" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with Giarda - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A31" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="46" t="s">
+        <v>425</v>
+      </c>
+      <c r="E31" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with Salmonella - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="48" x14ac:dyDescent="0.75">
+      <c r="A32" s="26" t="s">
+        <v>466</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="46" t="s">
+        <v>426</v>
+      </c>
+      <c r="E32" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v>% of people with Yersinia enterocolitica - Cases of disease prevalence per 100.000 inhabitants, per district, for each of the causes considered as relatable to the project</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08DA2C3-843D-4662-B2C7-78EB4A1DCF4E}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B49" sqref="A49:XFD49"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -5634,7 +8432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA67BB8F-F241-4238-A116-030260AF1676}">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
@@ -6713,15 +9511,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B580CB-20F4-4431-9AC1-C7F103128FA7}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED073F5-A8D3-49DE-9F2B-C279B45B9525}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G8"/>
+    <sheetView zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -6764,6 +9562,576 @@
     </row>
     <row r="2" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A2" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$8</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthMeasure</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C2" s="8" t="str">
+        <f>HealthMeasureOah!A2</f>
+        <v>site</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>HealthMeasureOah!D2</f>
+        <v>Sampling Site</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A3" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$8</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthMeasure</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C3" s="8" t="str">
+        <f>HealthMeasureOah!A3</f>
+        <v>site.identifier</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>HealthMeasureOah!D3</f>
+        <v>Site identifier</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A4" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$8</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthMeasure</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C4" s="8" t="str">
+        <f>HealthMeasureOah!A4</f>
+        <v>site.name</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f>HealthMeasureOah!D4</f>
+        <v>Site Name</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" s="6" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A5" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$8</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthMeasure</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C5" s="8" t="str">
+        <f>HealthMeasureOah!A5</f>
+        <v>site.gps</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f>HealthMeasureOah!D5</f>
+        <v>GPS</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F5" s="6" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A6" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$8</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthMeasure</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C6" s="8" t="str">
+        <f>HealthMeasureOah!A6</f>
+        <v>site.characteristics</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f>HealthMeasureOah!D6</f>
+        <v>Characteristics</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F6" s="6" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A7" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$8</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthMeasure</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>HealthMeasureOah!A7</f>
+        <v>dateOrPeriod[x]</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f>HealthMeasureOah!D7</f>
+        <v>Measure Date or Period</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A8" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$8</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthMeasure</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C8" s="8" t="str">
+        <f>HealthMeasureOah!A8</f>
+        <v>perfomer[x]</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>HealthMeasureOah!D8</f>
+        <v>Performer</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A9" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$8</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthMeasure</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>HealthMeasureOah!A9</f>
+        <v>type</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>HealthMeasureOah!D9</f>
+        <v>What is measured</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A10" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$8</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthMeasure</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C10" s="8" t="str">
+        <f>HealthMeasureOah!A10</f>
+        <v>result[x]</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>HealthMeasureOah!D10</f>
+        <v>Result</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A11" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$8</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthMeasure</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>491</v>
+      </c>
+      <c r="C11" s="8" t="str">
+        <f>HealthMeasureOah!A11</f>
+        <v>cohort</v>
+      </c>
+      <c r="D11" s="8" t="str">
+        <f>HealthMeasureOah!D11</f>
+        <v>Cohort</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A12" s="7" t="str">
+        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$8</f>
+        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/HealthMeasure</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C12" s="8" t="str">
+        <f>HealthMeasureOah!A11</f>
+        <v>cohort</v>
+      </c>
+      <c r="D12" s="8" t="str">
+        <f>HealthMeasureOah!D11</f>
+        <v>Cohort</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="C13"/>
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="C14"/>
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="C15"/>
+      <c r="D15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="C16"/>
+      <c r="D16"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C4567C37-90CE-47CE-8A0D-3B45C73FA168}"/>
+    <hyperlink ref="A1" r:id="rId2" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{1A84C05F-87C6-4A03-8243-A8AD37DB433C}"/>
+    <hyperlink ref="B3:B11" r:id="rId3" display="http://hl7.eu/fhir/ig/oah/StructureDefinition/observation-health-measure-oah" xr:uid="{E106BFBE-AF04-4846-86C2-F0592EA060B6}"/>
+    <hyperlink ref="B11" r:id="rId4" xr:uid="{F0EBE519-BC01-4182-A8A6-F3620EE66067}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{90A1F5D6-7E93-44F4-94C6-874EEB36C64E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4FF0EF7-8237-4091-A62C-388E6738FC80}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="23.31640625" customWidth="1"/>
+    <col min="5" max="5" width="35.08984375" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A6" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A7" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A8" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A9" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A10" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A11" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B580CB-20F4-4431-9AC1-C7F103128FA7}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="58.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.86328125" customWidth="1"/>
+    <col min="3" max="3" width="24.76953125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="31.2265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="31.2265625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A2" s="7" t="str">
         <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$3</f>
         <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/SimpleIndicator</v>
       </c>
@@ -6956,920 +10324,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8917C38-1E9C-4CA8-B026-1EC7F0AF7FE1}">
-  <sheetPr>
-    <tabColor theme="6" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="23.31640625" customWidth="1"/>
-    <col min="5" max="5" width="35.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A2" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A3" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A5" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A6" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A9AEBD-A9A0-493E-863C-D52F8723986B}">
-  <sheetPr>
-    <tabColor theme="7" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="58.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.86328125" customWidth="1"/>
-    <col min="3" max="3" width="76.76953125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.2265625" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="11.08984375" customWidth="1"/>
-    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A2" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="8" t="str">
-        <f>StructuredIndicatorOah!A2</f>
-        <v>sampleDetails</v>
-      </c>
-      <c r="D2" s="8" t="str">
-        <f>StructuredIndicatorOah!D2</f>
-        <v>Sample</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A3" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" s="8" t="str">
-        <f>StructuredIndicatorOah!A2</f>
-        <v>sampleDetails</v>
-      </c>
-      <c r="D3" s="8" t="str">
-        <f>StructuredIndicatorOah!D2</f>
-        <v>Sample</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A4" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" s="8" t="str">
-        <f>StructuredIndicatorOah!A2</f>
-        <v>sampleDetails</v>
-      </c>
-      <c r="D4" s="8" t="str">
-        <f>StructuredIndicatorOah!D2</f>
-        <v>Sample</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="F4" s="6" t="str">
-        <f>""</f>
-        <v/>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A5" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C5" s="8" t="str">
-        <f>StructuredIndicatorOah!A3</f>
-        <v>type</v>
-      </c>
-      <c r="D5" s="8" t="str">
-        <f>StructuredIndicatorOah!D3</f>
-        <v>What is measured</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="F5" s="6" t="str">
-        <f>""</f>
-        <v/>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A6" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C6" s="8" t="str">
-        <f>StructuredIndicatorOah!A4</f>
-        <v>date</v>
-      </c>
-      <c r="D6" s="8" t="str">
-        <f>StructuredIndicatorOah!D4</f>
-        <v>Observation date</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A7" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" s="8" t="str">
-        <f>StructuredIndicatorOah!A5</f>
-        <v>performer[x]</v>
-      </c>
-      <c r="D7" s="8" t="str">
-        <f>StructuredIndicatorOah!D5</f>
-        <v>Who made the measure</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A8" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C8" s="8" t="str">
-        <f>StructuredIndicatorOah!A6</f>
-        <v>component</v>
-      </c>
-      <c r="D8" s="8" t="str">
-        <f>StructuredIndicatorOah!D6</f>
-        <v>Component</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A9" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C9" s="8" t="str">
-        <f>StructuredIndicatorOah!A7</f>
-        <v>component.type</v>
-      </c>
-      <c r="D9" s="8" t="str">
-        <f>StructuredIndicatorOah!D7</f>
-        <v>What is measured</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A10" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$4</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/StructuredIndicator</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C10" s="8" t="str">
-        <f>StructuredIndicatorOah!A8</f>
-        <v>component.result[x]</v>
-      </c>
-      <c r="D10" s="8" t="str">
-        <f>StructuredIndicatorOah!D8</f>
-        <v>Result</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H10" s="8"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{0FD19491-9321-40B7-B0F0-8DD001375ACD}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8B5A90-6D36-45B7-9347-AA4594F3DFDD}">
-  <sheetPr>
-    <tabColor theme="6" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
-    <col min="3" max="3" width="36.2265625" customWidth="1"/>
-    <col min="4" max="4" width="39.6796875" customWidth="1"/>
-    <col min="5" max="5" width="35.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A2" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A3" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A5" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A6" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A7" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A8" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CAA406-B92E-4F33-947E-7872EDD03684}">
-  <sheetPr>
-    <tabColor theme="7" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:H12"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="A13:XFD13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <cols>
-    <col min="1" max="1" width="58.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.86328125" customWidth="1"/>
-    <col min="3" max="3" width="36" style="5" customWidth="1"/>
-    <col min="4" max="4" width="44.54296875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.2265625" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="11.08984375" customWidth="1"/>
-    <col min="8" max="8" width="37.54296875" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A2" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>299</v>
-      </c>
-      <c r="C2" s="8" t="str">
-        <f>SampleOah!A2</f>
-        <v>site</v>
-      </c>
-      <c r="D2" s="8" t="str">
-        <f>SampleOah!D2</f>
-        <v>Sampling Site</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A3" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="8" t="str">
-        <f>SampleOah!A2</f>
-        <v>site</v>
-      </c>
-      <c r="D3" s="8" t="str">
-        <f>SampleOah!D2</f>
-        <v>Sampling Site</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A4" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>299</v>
-      </c>
-      <c r="C4" s="27" t="str">
-        <f>SampleOah!A6</f>
-        <v>site.characteristics</v>
-      </c>
-      <c r="D4" s="27" t="str">
-        <f>SampleOah!D6</f>
-        <v>Characteristics</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A5" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>299</v>
-      </c>
-      <c r="C5" s="8" t="str">
-        <f>SampleOah!A8</f>
-        <v>dateOfSampling</v>
-      </c>
-      <c r="D5" s="8" t="str">
-        <f>SampleOah!D8</f>
-        <v>Date of Sample</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A6" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>299</v>
-      </c>
-      <c r="C6" s="8" t="str">
-        <f>SampleOah!A9</f>
-        <v>perfomer[x]</v>
-      </c>
-      <c r="D6" s="8" t="str">
-        <f>SampleOah!D9</f>
-        <v>Performer</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A7" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
-      </c>
-      <c r="B7" t="s">
-        <v>300</v>
-      </c>
-      <c r="C7" s="8" t="str">
-        <f>SampleOah!A2</f>
-        <v>site</v>
-      </c>
-      <c r="D7" s="8" t="str">
-        <f>SampleOah!D2</f>
-        <v>Sampling Site</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A8" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
-      </c>
-      <c r="B8" t="s">
-        <v>300</v>
-      </c>
-      <c r="C8" s="8" t="str">
-        <f>SampleOah!A3</f>
-        <v>site.identifier</v>
-      </c>
-      <c r="D8" s="8" t="str">
-        <f>SampleOah!D3</f>
-        <v>Site identifier</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A9" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
-      </c>
-      <c r="B9" t="s">
-        <v>300</v>
-      </c>
-      <c r="C9" s="8" t="str">
-        <f>SampleOah!A4</f>
-        <v>site.name</v>
-      </c>
-      <c r="D9" s="8" t="str">
-        <f>SampleOah!D4</f>
-        <v>Site Name</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A10" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
-      </c>
-      <c r="B10" t="s">
-        <v>300</v>
-      </c>
-      <c r="C10" s="8" t="str">
-        <f>SampleOah!A5</f>
-        <v>site.gps</v>
-      </c>
-      <c r="D10" s="8" t="str">
-        <f>SampleOah!D5</f>
-        <v>GPS</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A11" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
-      </c>
-      <c r="B11" t="s">
-        <v>300</v>
-      </c>
-      <c r="C11" s="27" t="str">
-        <f>SampleOah!A6</f>
-        <v>site.characteristics</v>
-      </c>
-      <c r="D11" s="27" t="str">
-        <f>SampleOah!D6</f>
-        <v>Characteristics</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A12" s="7" t="str">
-        <f>"http://hl7.eu/fhir/ig/oah/StructureDefinition/"&amp;LogicalModels!$A$5</f>
-        <v>http://hl7.eu/fhir/ig/oah/StructureDefinition/Sample</v>
-      </c>
-      <c r="B12" t="s">
-        <v>300</v>
-      </c>
-      <c r="C12" s="8" t="str">
-        <f>SampleOah!A7</f>
-        <v>site.formReference</v>
-      </c>
-      <c r="D12" s="8" t="str">
-        <f>SampleOah!D7</f>
-        <v>Form Reference</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="H12" s="8"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{E181CF34-81EF-44E5-98B8-1A9E617A5F12}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>